<commit_message>
fix: changed incorrect milestone date
</commit_message>
<xml_diff>
--- a/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
+++ b/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Documents\chadv1.0\chadv1.0\deliverables\timeline_and_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{7E7E4A59-A8CE-432B-B8DF-9C4B106A31BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF40E168-FA11-4ADA-9C64-EBF8F2ACC8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -492,7 +492,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,12 +580,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,7 +818,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -966,42 +960,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1011,19 +969,16 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,13 +1007,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1072,7 +1024,7 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1084,7 +1036,7 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1097,7 +1049,7 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1109,7 +1061,45 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1126,178 +1116,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -1487,6 +1306,38 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="5"/>
@@ -1499,15 +1350,42 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1650,15 +1528,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="38"/>
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="totalRow" dxfId="36"/>
-      <tableStyleElement type="firstColumn" dxfId="35"/>
-      <tableStyleElement type="lastColumn" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="secondRowStripe" dxfId="32"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="totalRow" dxfId="28"/>
+      <tableStyleElement type="firstColumn" dxfId="27"/>
+      <tableStyleElement type="lastColumn" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="25"/>
+      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="23"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2016,8 +1894,8 @@
   </sheetPr>
   <dimension ref="A1:DP54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2036,64 +1914,64 @@
     <row r="1" spans="1:120" ht="90" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="61">
+      <c r="Q1" s="100">
         <f>DATE(2025, 1, 17)</f>
         <v>45674</v>
       </c>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
     </row>
     <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="I2" s="62" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="I2" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="59">
+      <c r="Q2" s="98">
         <v>1</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
     </row>
     <row r="3" spans="1:120" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="20"/>
@@ -2103,182 +1981,182 @@
       <c r="A4" s="14"/>
       <c r="B4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="66">
+      <c r="I4" s="106">
         <f>I5</f>
         <v>45670</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64">
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="104">
         <f>P5</f>
         <v>45677</v>
       </c>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64">
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="104"/>
+      <c r="W4" s="104">
         <f>W5</f>
         <v>45684</v>
       </c>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64">
+      <c r="X4" s="104"/>
+      <c r="Y4" s="104"/>
+      <c r="Z4" s="104"/>
+      <c r="AA4" s="104"/>
+      <c r="AB4" s="104"/>
+      <c r="AC4" s="104"/>
+      <c r="AD4" s="104">
         <f>AD5</f>
         <v>45691</v>
       </c>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="64">
+      <c r="AE4" s="104"/>
+      <c r="AF4" s="104"/>
+      <c r="AG4" s="104"/>
+      <c r="AH4" s="104"/>
+      <c r="AI4" s="104"/>
+      <c r="AJ4" s="104"/>
+      <c r="AK4" s="104">
         <f>AK5</f>
         <v>45698</v>
       </c>
-      <c r="AL4" s="64"/>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="64"/>
-      <c r="AR4" s="64">
+      <c r="AL4" s="104"/>
+      <c r="AM4" s="104"/>
+      <c r="AN4" s="104"/>
+      <c r="AO4" s="104"/>
+      <c r="AP4" s="104"/>
+      <c r="AQ4" s="104"/>
+      <c r="AR4" s="104">
         <f>AR5</f>
         <v>45705</v>
       </c>
-      <c r="AS4" s="64"/>
-      <c r="AT4" s="64"/>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="64"/>
-      <c r="AY4" s="64">
+      <c r="AS4" s="104"/>
+      <c r="AT4" s="104"/>
+      <c r="AU4" s="104"/>
+      <c r="AV4" s="104"/>
+      <c r="AW4" s="104"/>
+      <c r="AX4" s="104"/>
+      <c r="AY4" s="104">
         <f>AY5</f>
         <v>45712</v>
       </c>
-      <c r="AZ4" s="64"/>
-      <c r="BA4" s="64"/>
-      <c r="BB4" s="64"/>
-      <c r="BC4" s="64"/>
-      <c r="BD4" s="64"/>
-      <c r="BE4" s="64"/>
-      <c r="BF4" s="64">
+      <c r="AZ4" s="104"/>
+      <c r="BA4" s="104"/>
+      <c r="BB4" s="104"/>
+      <c r="BC4" s="104"/>
+      <c r="BD4" s="104"/>
+      <c r="BE4" s="104"/>
+      <c r="BF4" s="104">
         <f>BF5</f>
         <v>45719</v>
       </c>
-      <c r="BG4" s="64"/>
-      <c r="BH4" s="64"/>
-      <c r="BI4" s="64"/>
-      <c r="BJ4" s="64"/>
-      <c r="BK4" s="64"/>
-      <c r="BL4" s="65"/>
-      <c r="BM4" s="64">
+      <c r="BG4" s="104"/>
+      <c r="BH4" s="104"/>
+      <c r="BI4" s="104"/>
+      <c r="BJ4" s="104"/>
+      <c r="BK4" s="104"/>
+      <c r="BL4" s="105"/>
+      <c r="BM4" s="104">
         <f>BM5</f>
         <v>45726</v>
       </c>
-      <c r="BN4" s="64"/>
-      <c r="BO4" s="64"/>
-      <c r="BP4" s="64"/>
-      <c r="BQ4" s="64"/>
-      <c r="BR4" s="64"/>
-      <c r="BS4" s="65"/>
-      <c r="BT4" s="64">
+      <c r="BN4" s="104"/>
+      <c r="BO4" s="104"/>
+      <c r="BP4" s="104"/>
+      <c r="BQ4" s="104"/>
+      <c r="BR4" s="104"/>
+      <c r="BS4" s="105"/>
+      <c r="BT4" s="104">
         <f>BT5</f>
         <v>45733</v>
       </c>
-      <c r="BU4" s="64"/>
-      <c r="BV4" s="64"/>
-      <c r="BW4" s="64"/>
-      <c r="BX4" s="64"/>
-      <c r="BY4" s="64"/>
-      <c r="BZ4" s="65"/>
-      <c r="CA4" s="64">
+      <c r="BU4" s="104"/>
+      <c r="BV4" s="104"/>
+      <c r="BW4" s="104"/>
+      <c r="BX4" s="104"/>
+      <c r="BY4" s="104"/>
+      <c r="BZ4" s="105"/>
+      <c r="CA4" s="104">
         <f>CA5</f>
         <v>45740</v>
       </c>
-      <c r="CB4" s="64"/>
-      <c r="CC4" s="64"/>
-      <c r="CD4" s="64"/>
-      <c r="CE4" s="64"/>
-      <c r="CF4" s="64"/>
-      <c r="CG4" s="65"/>
-      <c r="CH4" s="64">
+      <c r="CB4" s="104"/>
+      <c r="CC4" s="104"/>
+      <c r="CD4" s="104"/>
+      <c r="CE4" s="104"/>
+      <c r="CF4" s="104"/>
+      <c r="CG4" s="105"/>
+      <c r="CH4" s="104">
         <f>CH5</f>
         <v>45747</v>
       </c>
-      <c r="CI4" s="64"/>
-      <c r="CJ4" s="64"/>
-      <c r="CK4" s="64"/>
-      <c r="CL4" s="64"/>
-      <c r="CM4" s="64"/>
-      <c r="CN4" s="65"/>
-      <c r="CO4" s="64">
+      <c r="CI4" s="104"/>
+      <c r="CJ4" s="104"/>
+      <c r="CK4" s="104"/>
+      <c r="CL4" s="104"/>
+      <c r="CM4" s="104"/>
+      <c r="CN4" s="105"/>
+      <c r="CO4" s="104">
         <f>CO5</f>
         <v>45754</v>
       </c>
-      <c r="CP4" s="64"/>
-      <c r="CQ4" s="64"/>
-      <c r="CR4" s="64"/>
-      <c r="CS4" s="64"/>
-      <c r="CT4" s="64"/>
-      <c r="CU4" s="65"/>
-      <c r="CV4" s="64">
+      <c r="CP4" s="104"/>
+      <c r="CQ4" s="104"/>
+      <c r="CR4" s="104"/>
+      <c r="CS4" s="104"/>
+      <c r="CT4" s="104"/>
+      <c r="CU4" s="105"/>
+      <c r="CV4" s="104">
         <f>CV5</f>
         <v>45761</v>
       </c>
-      <c r="CW4" s="64"/>
-      <c r="CX4" s="64"/>
-      <c r="CY4" s="64"/>
-      <c r="CZ4" s="64"/>
-      <c r="DA4" s="64"/>
-      <c r="DB4" s="65"/>
-      <c r="DC4" s="64">
+      <c r="CW4" s="104"/>
+      <c r="CX4" s="104"/>
+      <c r="CY4" s="104"/>
+      <c r="CZ4" s="104"/>
+      <c r="DA4" s="104"/>
+      <c r="DB4" s="105"/>
+      <c r="DC4" s="104">
         <f>DC5</f>
         <v>45768</v>
       </c>
-      <c r="DD4" s="64"/>
-      <c r="DE4" s="64"/>
-      <c r="DF4" s="64"/>
-      <c r="DG4" s="64"/>
-      <c r="DH4" s="64"/>
-      <c r="DI4" s="65"/>
-      <c r="DJ4" s="64">
+      <c r="DD4" s="104"/>
+      <c r="DE4" s="104"/>
+      <c r="DF4" s="104"/>
+      <c r="DG4" s="104"/>
+      <c r="DH4" s="104"/>
+      <c r="DI4" s="105"/>
+      <c r="DJ4" s="104">
         <f>DJ5</f>
         <v>45775</v>
       </c>
-      <c r="DK4" s="64"/>
-      <c r="DL4" s="64"/>
-      <c r="DM4" s="64"/>
-      <c r="DN4" s="64"/>
-      <c r="DO4" s="64"/>
-      <c r="DP4" s="65"/>
+      <c r="DK4" s="104"/>
+      <c r="DL4" s="104"/>
+      <c r="DM4" s="104"/>
+      <c r="DN4" s="104"/>
+      <c r="DO4" s="104"/>
+      <c r="DP4" s="105"/>
     </row>
     <row r="5" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54" t="s">
+      <c r="A5" s="92"/>
+      <c r="B5" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="97" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="24">
@@ -2731,12 +2609,12 @@
       </c>
     </row>
     <row r="6" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="53"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
       <c r="I6" s="27" t="str">
         <f t="shared" ref="I6:AN6" si="43">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -3258,13 +3136,13 @@
     </row>
     <row r="8" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14"/>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="83"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
         <f t="shared" ref="H8:H51" si="51">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -3329,17 +3207,17 @@
     </row>
     <row r="9" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14"/>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="75">
+      <c r="C9" s="59"/>
+      <c r="D9" s="60">
         <v>1</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="61">
         <v>45674</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="61">
         <v>45674</v>
       </c>
       <c r="G9" s="17"/>
@@ -3348,7 +3226,7 @@
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="77"/>
+      <c r="M9" s="62"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
@@ -3459,19 +3337,19 @@
     </row>
     <row r="10" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="88">
+      <c r="D10" s="72">
         <v>1</v>
       </c>
-      <c r="E10" s="89">
+      <c r="E10" s="73">
         <v>45677</v>
       </c>
-      <c r="F10" s="89">
+      <c r="F10" s="73">
         <f>E10+4</f>
         <v>45681</v>
       </c>
@@ -3487,11 +3365,11 @@
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
       <c r="U10" s="37"/>
       <c r="V10" s="37"/>
       <c r="W10" s="37"/>
@@ -3595,10 +3473,10 @@
     </row>
     <row r="11" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14"/>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="38">
@@ -3732,19 +3610,19 @@
     </row>
     <row r="12" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14"/>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="60">
         <v>1</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="61">
         <v>45688</v>
       </c>
-      <c r="F12" s="76">
+      <c r="F12" s="61">
         <v>45688</v>
       </c>
       <c r="G12" s="17"/>
@@ -3767,7 +3645,7 @@
       <c r="X12" s="37"/>
       <c r="Y12" s="37"/>
       <c r="Z12" s="37"/>
-      <c r="AA12" s="77"/>
+      <c r="AA12" s="62"/>
       <c r="AB12" s="37"/>
       <c r="AC12" s="37"/>
       <c r="AD12" s="37"/>
@@ -3864,20 +3742,20 @@
     </row>
     <row r="13" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="82">
         <v>1</v>
       </c>
-      <c r="E13" s="99">
+      <c r="E13" s="83">
         <f>F11</f>
         <v>45688</v>
       </c>
-      <c r="F13" s="99">
+      <c r="F13" s="83">
         <f>E13+7</f>
         <v>45695</v>
       </c>
@@ -3904,14 +3782,14 @@
       <c r="X13" s="37"/>
       <c r="Y13" s="37"/>
       <c r="Z13" s="37"/>
-      <c r="AA13" s="91"/>
-      <c r="AB13" s="91"/>
-      <c r="AC13" s="91"/>
-      <c r="AD13" s="91"/>
-      <c r="AE13" s="91"/>
-      <c r="AF13" s="91"/>
-      <c r="AG13" s="91"/>
-      <c r="AH13" s="91"/>
+      <c r="AA13" s="75"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="75"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="75"/>
+      <c r="AG13" s="75"/>
+      <c r="AH13" s="75"/>
       <c r="AI13" s="37"/>
       <c r="AJ13" s="37"/>
       <c r="AK13" s="37"/>
@@ -4001,19 +3879,19 @@
     </row>
     <row r="14" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13"/>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="75">
+      <c r="D14" s="60">
         <v>0</v>
       </c>
-      <c r="E14" s="76">
+      <c r="E14" s="61">
         <v>45695</v>
       </c>
-      <c r="F14" s="76">
+      <c r="F14" s="61">
         <v>45695</v>
       </c>
       <c r="G14" s="17"/>
@@ -4043,7 +3921,7 @@
       <c r="AE14" s="37"/>
       <c r="AF14" s="37"/>
       <c r="AG14" s="37"/>
-      <c r="AH14" s="78"/>
+      <c r="AH14" s="63"/>
       <c r="AI14" s="37"/>
       <c r="AJ14" s="37"/>
       <c r="AK14" s="37"/>
@@ -4133,20 +4011,20 @@
     </row>
     <row r="15" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13"/>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="82">
         <v>0</v>
       </c>
-      <c r="E15" s="99">
+      <c r="E15" s="83">
         <f>F13</f>
         <v>45695</v>
       </c>
-      <c r="F15" s="99">
+      <c r="F15" s="83">
         <f>E15+7</f>
         <v>45702</v>
       </c>
@@ -4180,14 +4058,14 @@
       <c r="AE15" s="37"/>
       <c r="AF15" s="37"/>
       <c r="AG15" s="37"/>
-      <c r="AH15" s="100"/>
-      <c r="AI15" s="100"/>
-      <c r="AJ15" s="100"/>
-      <c r="AK15" s="100"/>
-      <c r="AL15" s="100"/>
-      <c r="AM15" s="100"/>
-      <c r="AN15" s="100"/>
-      <c r="AO15" s="100"/>
+      <c r="AH15" s="84"/>
+      <c r="AI15" s="84"/>
+      <c r="AJ15" s="84"/>
+      <c r="AK15" s="84"/>
+      <c r="AL15" s="84"/>
+      <c r="AM15" s="84"/>
+      <c r="AN15" s="84"/>
+      <c r="AO15" s="84"/>
       <c r="AP15" s="37"/>
       <c r="AQ15" s="37"/>
       <c r="AR15" s="37"/>
@@ -4270,19 +4148,19 @@
     </row>
     <row r="16" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="13"/>
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="72">
         <v>0</v>
       </c>
-      <c r="E16" s="89">
+      <c r="E16" s="73">
         <v>45695</v>
       </c>
-      <c r="F16" s="89">
+      <c r="F16" s="73">
         <v>45702</v>
       </c>
       <c r="G16" s="17"/>
@@ -4312,14 +4190,14 @@
       <c r="AE16" s="37"/>
       <c r="AF16" s="37"/>
       <c r="AG16" s="37"/>
-      <c r="AH16" s="105"/>
-      <c r="AI16" s="105"/>
-      <c r="AJ16" s="105"/>
-      <c r="AK16" s="105"/>
-      <c r="AL16" s="105"/>
-      <c r="AM16" s="105"/>
-      <c r="AN16" s="105"/>
-      <c r="AO16" s="105"/>
+      <c r="AH16" s="89"/>
+      <c r="AI16" s="89"/>
+      <c r="AJ16" s="89"/>
+      <c r="AK16" s="89"/>
+      <c r="AL16" s="89"/>
+      <c r="AM16" s="89"/>
+      <c r="AN16" s="89"/>
+      <c r="AO16" s="89"/>
       <c r="AP16" s="37"/>
       <c r="AQ16" s="37"/>
       <c r="AR16" s="37"/>
@@ -4402,10 +4280,10 @@
     </row>
     <row r="17" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13"/>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="56" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="35">
@@ -4415,7 +4293,7 @@
         <v>45695</v>
       </c>
       <c r="F17" s="36">
-        <v>45695</v>
+        <v>45702</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5"/>
@@ -4444,14 +4322,14 @@
       <c r="AE17" s="37"/>
       <c r="AF17" s="37"/>
       <c r="AG17" s="37"/>
-      <c r="AH17" s="106"/>
-      <c r="AI17" s="106"/>
-      <c r="AJ17" s="106"/>
-      <c r="AK17" s="106"/>
-      <c r="AL17" s="106"/>
-      <c r="AM17" s="106"/>
-      <c r="AN17" s="106"/>
-      <c r="AO17" s="106"/>
+      <c r="AH17" s="90"/>
+      <c r="AI17" s="90"/>
+      <c r="AJ17" s="90"/>
+      <c r="AK17" s="90"/>
+      <c r="AL17" s="90"/>
+      <c r="AM17" s="90"/>
+      <c r="AN17" s="90"/>
+      <c r="AO17" s="90"/>
       <c r="AP17" s="37"/>
       <c r="AQ17" s="37"/>
       <c r="AR17" s="37"/>
@@ -4534,19 +4412,19 @@
     </row>
     <row r="18" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="13"/>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="75">
+      <c r="D18" s="60">
         <v>0</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="61">
         <v>45702</v>
       </c>
-      <c r="F18" s="76">
+      <c r="F18" s="61">
         <v>45702</v>
       </c>
       <c r="G18" s="17"/>
@@ -4583,7 +4461,7 @@
       <c r="AL18" s="37"/>
       <c r="AM18" s="37"/>
       <c r="AN18" s="37"/>
-      <c r="AO18" s="78"/>
+      <c r="AO18" s="63"/>
       <c r="AP18" s="37"/>
       <c r="AQ18" s="37"/>
       <c r="AR18" s="37"/>
@@ -4666,10 +4544,10 @@
     </row>
     <row r="19" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13"/>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="38">
@@ -4800,19 +4678,19 @@
     </row>
     <row r="20" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13"/>
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="93" t="s">
+      <c r="C20" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="94">
+      <c r="D20" s="78">
         <v>0</v>
       </c>
-      <c r="E20" s="95">
+      <c r="E20" s="79">
         <v>45702</v>
       </c>
-      <c r="F20" s="95">
+      <c r="F20" s="79">
         <v>45709</v>
       </c>
       <c r="G20" s="17"/>
@@ -4849,14 +4727,14 @@
       <c r="AL20" s="37"/>
       <c r="AM20" s="37"/>
       <c r="AN20" s="37"/>
-      <c r="AO20" s="100"/>
-      <c r="AP20" s="100"/>
-      <c r="AQ20" s="100"/>
-      <c r="AR20" s="100"/>
-      <c r="AS20" s="100"/>
-      <c r="AT20" s="100"/>
-      <c r="AU20" s="100"/>
-      <c r="AV20" s="100"/>
+      <c r="AO20" s="84"/>
+      <c r="AP20" s="84"/>
+      <c r="AQ20" s="84"/>
+      <c r="AR20" s="84"/>
+      <c r="AS20" s="84"/>
+      <c r="AT20" s="84"/>
+      <c r="AU20" s="84"/>
+      <c r="AV20" s="84"/>
       <c r="AW20" s="37"/>
       <c r="AX20" s="37"/>
       <c r="AY20" s="37"/>
@@ -4932,19 +4810,19 @@
     </row>
     <row r="21" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="13"/>
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="88">
+      <c r="D21" s="72">
         <v>0</v>
       </c>
-      <c r="E21" s="89">
+      <c r="E21" s="73">
         <v>45702</v>
       </c>
-      <c r="F21" s="89">
+      <c r="F21" s="73">
         <v>45709</v>
       </c>
       <c r="G21" s="17"/>
@@ -4981,14 +4859,14 @@
       <c r="AL21" s="37"/>
       <c r="AM21" s="37"/>
       <c r="AN21" s="37"/>
-      <c r="AO21" s="107"/>
-      <c r="AP21" s="107"/>
-      <c r="AQ21" s="107"/>
-      <c r="AR21" s="107"/>
-      <c r="AS21" s="107"/>
-      <c r="AT21" s="107"/>
-      <c r="AU21" s="107"/>
-      <c r="AV21" s="107"/>
+      <c r="AO21" s="91"/>
+      <c r="AP21" s="91"/>
+      <c r="AQ21" s="91"/>
+      <c r="AR21" s="91"/>
+      <c r="AS21" s="91"/>
+      <c r="AT21" s="91"/>
+      <c r="AU21" s="91"/>
+      <c r="AV21" s="91"/>
       <c r="AW21" s="37"/>
       <c r="AX21" s="37"/>
       <c r="AY21" s="37"/>
@@ -5064,19 +4942,19 @@
     </row>
     <row r="22" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="75">
+      <c r="D22" s="60">
         <v>0</v>
       </c>
-      <c r="E22" s="76">
+      <c r="E22" s="61">
         <v>45709</v>
       </c>
-      <c r="F22" s="76">
+      <c r="F22" s="61">
         <v>45709</v>
       </c>
       <c r="G22" s="17"/>
@@ -5120,7 +4998,7 @@
       <c r="AS22" s="37"/>
       <c r="AT22" s="37"/>
       <c r="AU22" s="37"/>
-      <c r="AV22" s="78"/>
+      <c r="AV22" s="63"/>
       <c r="AW22" s="37"/>
       <c r="AX22" s="37"/>
       <c r="AY22" s="37"/>
@@ -5196,20 +5074,20 @@
     </row>
     <row r="23" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="13"/>
-      <c r="B23" s="101" t="s">
+      <c r="B23" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="103">
+      <c r="D23" s="87">
         <v>0</v>
       </c>
-      <c r="E23" s="104">
+      <c r="E23" s="88">
         <f>F19</f>
         <v>45709</v>
       </c>
-      <c r="F23" s="104">
+      <c r="F23" s="88">
         <f>E23+7</f>
         <v>45716</v>
       </c>
@@ -5254,14 +5132,14 @@
       <c r="AS23" s="37"/>
       <c r="AT23" s="37"/>
       <c r="AU23" s="37"/>
-      <c r="AV23" s="107"/>
-      <c r="AW23" s="107"/>
-      <c r="AX23" s="107"/>
-      <c r="AY23" s="107"/>
-      <c r="AZ23" s="107"/>
-      <c r="BA23" s="107"/>
-      <c r="BB23" s="107"/>
-      <c r="BC23" s="107"/>
+      <c r="AV23" s="91"/>
+      <c r="AW23" s="91"/>
+      <c r="AX23" s="91"/>
+      <c r="AY23" s="91"/>
+      <c r="AZ23" s="91"/>
+      <c r="BA23" s="91"/>
+      <c r="BB23" s="91"/>
+      <c r="BC23" s="91"/>
       <c r="BD23" s="37"/>
       <c r="BE23" s="37"/>
       <c r="BF23" s="37"/>
@@ -5330,19 +5208,19 @@
     </row>
     <row r="24" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="13"/>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="93" t="s">
+      <c r="C24" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="94">
+      <c r="D24" s="78">
         <v>0</v>
       </c>
-      <c r="E24" s="95">
+      <c r="E24" s="79">
         <v>45709</v>
       </c>
-      <c r="F24" s="95">
+      <c r="F24" s="79">
         <v>45716</v>
       </c>
       <c r="G24" s="17"/>
@@ -5386,14 +5264,14 @@
       <c r="AS24" s="37"/>
       <c r="AT24" s="37"/>
       <c r="AU24" s="37"/>
-      <c r="AV24" s="100"/>
-      <c r="AW24" s="100"/>
-      <c r="AX24" s="100"/>
-      <c r="AY24" s="100"/>
-      <c r="AZ24" s="100"/>
-      <c r="BA24" s="100"/>
-      <c r="BB24" s="100"/>
-      <c r="BC24" s="100"/>
+      <c r="AV24" s="84"/>
+      <c r="AW24" s="84"/>
+      <c r="AX24" s="84"/>
+      <c r="AY24" s="84"/>
+      <c r="AZ24" s="84"/>
+      <c r="BA24" s="84"/>
+      <c r="BB24" s="84"/>
+      <c r="BC24" s="84"/>
       <c r="BD24" s="37"/>
       <c r="BE24" s="37"/>
       <c r="BF24" s="37"/>
@@ -5462,10 +5340,10 @@
     </row>
     <row r="25" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="13"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="56" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="35">
@@ -5518,14 +5396,14 @@
       <c r="AS25" s="37"/>
       <c r="AT25" s="37"/>
       <c r="AU25" s="37"/>
-      <c r="AV25" s="106"/>
-      <c r="AW25" s="106"/>
-      <c r="AX25" s="106"/>
-      <c r="AY25" s="106"/>
-      <c r="AZ25" s="106"/>
-      <c r="BA25" s="106"/>
-      <c r="BB25" s="106"/>
-      <c r="BC25" s="106"/>
+      <c r="AV25" s="90"/>
+      <c r="AW25" s="90"/>
+      <c r="AX25" s="90"/>
+      <c r="AY25" s="90"/>
+      <c r="AZ25" s="90"/>
+      <c r="BA25" s="90"/>
+      <c r="BB25" s="90"/>
+      <c r="BC25" s="90"/>
       <c r="BD25" s="37"/>
       <c r="BE25" s="37"/>
       <c r="BF25" s="37"/>
@@ -5594,19 +5472,19 @@
     </row>
     <row r="26" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="13"/>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="75">
+      <c r="D26" s="60">
         <v>0</v>
       </c>
-      <c r="E26" s="76">
+      <c r="E26" s="61">
         <v>45716</v>
       </c>
-      <c r="F26" s="76">
+      <c r="F26" s="61">
         <v>45716</v>
       </c>
       <c r="G26" s="17"/>
@@ -5657,7 +5535,7 @@
       <c r="AZ26" s="37"/>
       <c r="BA26" s="37"/>
       <c r="BB26" s="37"/>
-      <c r="BC26" s="78"/>
+      <c r="BC26" s="63"/>
       <c r="BD26" s="37"/>
       <c r="BE26" s="37"/>
       <c r="BF26" s="37"/>
@@ -5726,10 +5604,10 @@
     </row>
     <row r="27" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="13"/>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="38">
@@ -5860,20 +5738,20 @@
     </row>
     <row r="28" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="13"/>
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="102" t="s">
+      <c r="C28" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="103">
+      <c r="D28" s="87">
         <v>0</v>
       </c>
-      <c r="E28" s="104">
+      <c r="E28" s="88">
         <f>F26</f>
         <v>45716</v>
       </c>
-      <c r="F28" s="104">
+      <c r="F28" s="88">
         <f>E28+7</f>
         <v>45723</v>
       </c>
@@ -5925,14 +5803,14 @@
       <c r="AZ28" s="37"/>
       <c r="BA28" s="37"/>
       <c r="BB28" s="37"/>
-      <c r="BC28" s="108"/>
-      <c r="BD28" s="108"/>
-      <c r="BE28" s="108"/>
-      <c r="BF28" s="108"/>
-      <c r="BG28" s="108"/>
-      <c r="BH28" s="108"/>
-      <c r="BI28" s="108"/>
-      <c r="BJ28" s="108"/>
+      <c r="BC28" s="91"/>
+      <c r="BD28" s="91"/>
+      <c r="BE28" s="91"/>
+      <c r="BF28" s="91"/>
+      <c r="BG28" s="91"/>
+      <c r="BH28" s="91"/>
+      <c r="BI28" s="91"/>
+      <c r="BJ28" s="91"/>
       <c r="BK28" s="37"/>
       <c r="BL28" s="37"/>
       <c r="BM28" s="37"/>
@@ -5994,19 +5872,19 @@
     </row>
     <row r="29" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="13"/>
-      <c r="B29" s="96" t="s">
+      <c r="B29" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="97" t="s">
+      <c r="C29" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="98">
+      <c r="D29" s="82">
         <v>0</v>
       </c>
-      <c r="E29" s="99">
+      <c r="E29" s="83">
         <v>45716</v>
       </c>
-      <c r="F29" s="99">
+      <c r="F29" s="83">
         <v>45723</v>
       </c>
       <c r="G29" s="17"/>
@@ -6057,14 +5935,14 @@
       <c r="AZ29" s="37"/>
       <c r="BA29" s="37"/>
       <c r="BB29" s="37"/>
-      <c r="BC29" s="100"/>
-      <c r="BD29" s="100"/>
-      <c r="BE29" s="100"/>
-      <c r="BF29" s="100"/>
-      <c r="BG29" s="100"/>
-      <c r="BH29" s="100"/>
-      <c r="BI29" s="100"/>
-      <c r="BJ29" s="100"/>
+      <c r="BC29" s="84"/>
+      <c r="BD29" s="84"/>
+      <c r="BE29" s="84"/>
+      <c r="BF29" s="84"/>
+      <c r="BG29" s="84"/>
+      <c r="BH29" s="84"/>
+      <c r="BI29" s="84"/>
+      <c r="BJ29" s="84"/>
       <c r="BK29" s="37"/>
       <c r="BL29" s="37"/>
       <c r="BM29" s="37"/>
@@ -6126,20 +6004,20 @@
     </row>
     <row r="30" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="13"/>
-      <c r="B30" s="96" t="s">
+      <c r="B30" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="97" t="s">
+      <c r="C30" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="98">
+      <c r="D30" s="82">
         <v>0</v>
       </c>
-      <c r="E30" s="99">
+      <c r="E30" s="83">
         <f>F27</f>
         <v>45723</v>
       </c>
-      <c r="F30" s="99">
+      <c r="F30" s="83">
         <f>E30+7</f>
         <v>45730</v>
       </c>
@@ -6198,14 +6076,14 @@
       <c r="BG30" s="37"/>
       <c r="BH30" s="37"/>
       <c r="BI30" s="37"/>
-      <c r="BJ30" s="100"/>
-      <c r="BK30" s="100"/>
-      <c r="BL30" s="100"/>
-      <c r="BM30" s="100"/>
-      <c r="BN30" s="100"/>
-      <c r="BO30" s="100"/>
-      <c r="BP30" s="100"/>
-      <c r="BQ30" s="100"/>
+      <c r="BJ30" s="84"/>
+      <c r="BK30" s="84"/>
+      <c r="BL30" s="84"/>
+      <c r="BM30" s="84"/>
+      <c r="BN30" s="84"/>
+      <c r="BO30" s="84"/>
+      <c r="BP30" s="84"/>
+      <c r="BQ30" s="84"/>
       <c r="BR30" s="37"/>
       <c r="BS30" s="37"/>
       <c r="BT30" s="37"/>
@@ -6260,19 +6138,19 @@
     </row>
     <row r="31" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="13"/>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="102" t="s">
+      <c r="C31" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="103">
+      <c r="D31" s="87">
         <v>0</v>
       </c>
-      <c r="E31" s="104">
+      <c r="E31" s="88">
         <v>45723</v>
       </c>
-      <c r="F31" s="104">
+      <c r="F31" s="88">
         <v>45730</v>
       </c>
       <c r="G31" s="17"/>
@@ -6330,14 +6208,14 @@
       <c r="BG31" s="37"/>
       <c r="BH31" s="37"/>
       <c r="BI31" s="37"/>
-      <c r="BJ31" s="108"/>
-      <c r="BK31" s="108"/>
-      <c r="BL31" s="108"/>
-      <c r="BM31" s="108"/>
-      <c r="BN31" s="108"/>
-      <c r="BO31" s="108"/>
-      <c r="BP31" s="108"/>
-      <c r="BQ31" s="108"/>
+      <c r="BJ31" s="91"/>
+      <c r="BK31" s="91"/>
+      <c r="BL31" s="91"/>
+      <c r="BM31" s="91"/>
+      <c r="BN31" s="91"/>
+      <c r="BO31" s="91"/>
+      <c r="BP31" s="91"/>
+      <c r="BQ31" s="91"/>
       <c r="BR31" s="37"/>
       <c r="BS31" s="37"/>
       <c r="BT31" s="37"/>
@@ -6392,10 +6270,10 @@
     </row>
     <row r="32" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="13"/>
-      <c r="B32" s="69" t="s">
+      <c r="B32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="38">
@@ -6524,10 +6402,10 @@
     </row>
     <row r="33" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="13"/>
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="38">
@@ -6656,19 +6534,19 @@
     </row>
     <row r="34" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="13"/>
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="97" t="s">
+      <c r="C34" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="98">
+      <c r="D34" s="82">
         <v>0</v>
       </c>
-      <c r="E34" s="99">
+      <c r="E34" s="83">
         <v>45730</v>
       </c>
-      <c r="F34" s="99">
+      <c r="F34" s="83">
         <v>45737</v>
       </c>
       <c r="G34" s="17"/>
@@ -6733,14 +6611,14 @@
       <c r="BN34" s="37"/>
       <c r="BO34" s="37"/>
       <c r="BP34" s="37"/>
-      <c r="BQ34" s="100"/>
-      <c r="BR34" s="100"/>
-      <c r="BS34" s="100"/>
-      <c r="BT34" s="100"/>
-      <c r="BU34" s="100"/>
-      <c r="BV34" s="100"/>
-      <c r="BW34" s="100"/>
-      <c r="BX34" s="100"/>
+      <c r="BQ34" s="84"/>
+      <c r="BR34" s="84"/>
+      <c r="BS34" s="84"/>
+      <c r="BT34" s="84"/>
+      <c r="BU34" s="84"/>
+      <c r="BV34" s="84"/>
+      <c r="BW34" s="84"/>
+      <c r="BX34" s="84"/>
       <c r="BY34" s="37"/>
       <c r="BZ34" s="37"/>
       <c r="CA34" s="37"/>
@@ -6788,19 +6666,19 @@
     </row>
     <row r="35" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="13"/>
-      <c r="B35" s="101" t="s">
+      <c r="B35" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="102" t="s">
+      <c r="C35" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="103">
+      <c r="D35" s="87">
         <v>0</v>
       </c>
-      <c r="E35" s="104">
+      <c r="E35" s="88">
         <v>45730</v>
       </c>
-      <c r="F35" s="104">
+      <c r="F35" s="88">
         <v>45737</v>
       </c>
       <c r="G35" s="17"/>
@@ -6865,14 +6743,14 @@
       <c r="BN35" s="37"/>
       <c r="BO35" s="37"/>
       <c r="BP35" s="37"/>
-      <c r="BQ35" s="108"/>
-      <c r="BR35" s="108"/>
-      <c r="BS35" s="108"/>
-      <c r="BT35" s="108"/>
-      <c r="BU35" s="108"/>
-      <c r="BV35" s="108"/>
-      <c r="BW35" s="108"/>
-      <c r="BX35" s="108"/>
+      <c r="BQ35" s="91"/>
+      <c r="BR35" s="91"/>
+      <c r="BS35" s="91"/>
+      <c r="BT35" s="91"/>
+      <c r="BU35" s="91"/>
+      <c r="BV35" s="91"/>
+      <c r="BW35" s="91"/>
+      <c r="BX35" s="91"/>
       <c r="BY35" s="37"/>
       <c r="BZ35" s="37"/>
       <c r="CA35" s="37"/>
@@ -6920,10 +6798,10 @@
     </row>
     <row r="36" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="13"/>
-      <c r="B36" s="69" t="s">
+      <c r="B36" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="38">
@@ -7054,19 +6932,19 @@
     </row>
     <row r="37" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="13"/>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="74" t="s">
+      <c r="C37" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="75">
+      <c r="D37" s="60">
         <v>0</v>
       </c>
-      <c r="E37" s="76">
+      <c r="E37" s="61">
         <v>45737</v>
       </c>
-      <c r="F37" s="76">
+      <c r="F37" s="61">
         <v>45737</v>
       </c>
       <c r="G37" s="17"/>
@@ -7138,7 +7016,7 @@
       <c r="BU37" s="37"/>
       <c r="BV37" s="37"/>
       <c r="BW37" s="37"/>
-      <c r="BX37" s="78"/>
+      <c r="BX37" s="63"/>
       <c r="BY37" s="37"/>
       <c r="BZ37" s="37"/>
       <c r="CA37" s="37"/>
@@ -7186,10 +7064,10 @@
     </row>
     <row r="38" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="71" t="s">
+      <c r="C38" s="56" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="35">
@@ -7318,19 +7196,19 @@
     </row>
     <row r="39" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="13"/>
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="87" t="s">
+      <c r="C39" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="72">
         <v>0</v>
       </c>
-      <c r="E39" s="89">
+      <c r="E39" s="73">
         <v>45737</v>
       </c>
-      <c r="F39" s="89">
+      <c r="F39" s="73">
         <v>45744</v>
       </c>
       <c r="G39" s="17"/>
@@ -7402,14 +7280,14 @@
       <c r="BU39" s="37"/>
       <c r="BV39" s="37"/>
       <c r="BW39" s="37"/>
-      <c r="BX39" s="108"/>
-      <c r="BY39" s="108"/>
-      <c r="BZ39" s="108"/>
-      <c r="CA39" s="108"/>
-      <c r="CB39" s="108"/>
-      <c r="CC39" s="108"/>
-      <c r="CD39" s="108"/>
-      <c r="CE39" s="108"/>
+      <c r="BX39" s="91"/>
+      <c r="BY39" s="91"/>
+      <c r="BZ39" s="91"/>
+      <c r="CA39" s="91"/>
+      <c r="CB39" s="91"/>
+      <c r="CC39" s="91"/>
+      <c r="CD39" s="91"/>
+      <c r="CE39" s="91"/>
       <c r="CF39" s="37"/>
       <c r="CG39" s="37"/>
       <c r="CH39" s="37"/>
@@ -7450,20 +7328,20 @@
     </row>
     <row r="40" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="13"/>
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="97" t="s">
+      <c r="C40" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="98">
+      <c r="D40" s="82">
         <v>0</v>
       </c>
-      <c r="E40" s="99">
+      <c r="E40" s="83">
         <f>F36</f>
         <v>45737</v>
       </c>
-      <c r="F40" s="99">
+      <c r="F40" s="83">
         <f>E40+7</f>
         <v>45744</v>
       </c>
@@ -7536,14 +7414,14 @@
       <c r="BU40" s="37"/>
       <c r="BV40" s="37"/>
       <c r="BW40" s="37"/>
-      <c r="BX40" s="100"/>
-      <c r="BY40" s="100"/>
-      <c r="BZ40" s="100"/>
-      <c r="CA40" s="100"/>
-      <c r="CB40" s="100"/>
-      <c r="CC40" s="100"/>
-      <c r="CD40" s="100"/>
-      <c r="CE40" s="100"/>
+      <c r="BX40" s="84"/>
+      <c r="BY40" s="84"/>
+      <c r="BZ40" s="84"/>
+      <c r="CA40" s="84"/>
+      <c r="CB40" s="84"/>
+      <c r="CC40" s="84"/>
+      <c r="CD40" s="84"/>
+      <c r="CE40" s="84"/>
       <c r="CF40" s="37"/>
       <c r="CG40" s="37"/>
       <c r="CH40" s="37"/>
@@ -7584,19 +7462,19 @@
     </row>
     <row r="41" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="13"/>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="74" t="s">
+      <c r="C41" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="75">
+      <c r="D41" s="60">
         <v>0</v>
       </c>
-      <c r="E41" s="76">
+      <c r="E41" s="61">
         <v>45744</v>
       </c>
-      <c r="F41" s="76">
+      <c r="F41" s="61">
         <v>45744</v>
       </c>
       <c r="G41" s="17"/>
@@ -7674,7 +7552,7 @@
       <c r="CB41" s="37"/>
       <c r="CC41" s="40"/>
       <c r="CD41" s="37"/>
-      <c r="CE41" s="78"/>
+      <c r="CE41" s="63"/>
       <c r="CF41" s="37"/>
       <c r="CG41" s="37"/>
       <c r="CH41" s="37"/>
@@ -7715,20 +7593,20 @@
     </row>
     <row r="42" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="13"/>
-      <c r="B42" s="96" t="s">
+      <c r="B42" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="97" t="s">
+      <c r="C42" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="98">
+      <c r="D42" s="82">
         <v>0</v>
       </c>
-      <c r="E42" s="99">
+      <c r="E42" s="83">
         <f>F40</f>
         <v>45744</v>
       </c>
-      <c r="F42" s="99">
+      <c r="F42" s="83">
         <f>E42+7</f>
         <v>45751</v>
       </c>
@@ -7807,14 +7685,14 @@
       <c r="CB42" s="37"/>
       <c r="CC42" s="40"/>
       <c r="CD42" s="37"/>
-      <c r="CE42" s="100"/>
-      <c r="CF42" s="100"/>
-      <c r="CG42" s="100"/>
-      <c r="CH42" s="100"/>
-      <c r="CI42" s="100"/>
-      <c r="CJ42" s="100"/>
-      <c r="CK42" s="100"/>
-      <c r="CL42" s="100"/>
+      <c r="CE42" s="84"/>
+      <c r="CF42" s="84"/>
+      <c r="CG42" s="84"/>
+      <c r="CH42" s="84"/>
+      <c r="CI42" s="84"/>
+      <c r="CJ42" s="84"/>
+      <c r="CK42" s="84"/>
+      <c r="CL42" s="84"/>
       <c r="CM42" s="37"/>
       <c r="CN42" s="37"/>
       <c r="CO42" s="37"/>
@@ -7848,10 +7726,10 @@
     </row>
     <row r="43" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="13"/>
-      <c r="B43" s="69" t="s">
+      <c r="B43" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="72" t="s">
+      <c r="C43" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D43" s="38">
@@ -7980,20 +7858,20 @@
     </row>
     <row r="44" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="13"/>
-      <c r="B44" s="101" t="s">
+      <c r="B44" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="102" t="s">
+      <c r="C44" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="103">
+      <c r="D44" s="87">
         <v>0</v>
       </c>
-      <c r="E44" s="104">
+      <c r="E44" s="88">
         <f>F42</f>
         <v>45751</v>
       </c>
-      <c r="F44" s="104">
+      <c r="F44" s="88">
         <f>E44+7</f>
         <v>45758</v>
       </c>
@@ -8080,14 +7958,14 @@
       <c r="CI44" s="37"/>
       <c r="CJ44" s="37"/>
       <c r="CK44" s="37"/>
-      <c r="CL44" s="108"/>
-      <c r="CM44" s="108"/>
-      <c r="CN44" s="108"/>
-      <c r="CO44" s="108"/>
-      <c r="CP44" s="108"/>
-      <c r="CQ44" s="108"/>
-      <c r="CR44" s="108"/>
-      <c r="CS44" s="108"/>
+      <c r="CL44" s="91"/>
+      <c r="CM44" s="91"/>
+      <c r="CN44" s="91"/>
+      <c r="CO44" s="91"/>
+      <c r="CP44" s="91"/>
+      <c r="CQ44" s="91"/>
+      <c r="CR44" s="91"/>
+      <c r="CS44" s="91"/>
       <c r="CT44" s="37"/>
       <c r="CU44" s="37"/>
       <c r="CV44" s="37"/>
@@ -8114,19 +7992,19 @@
     </row>
     <row r="45" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="13"/>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="C45" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="75">
+      <c r="D45" s="60">
         <v>0</v>
       </c>
-      <c r="E45" s="76">
+      <c r="E45" s="61">
         <v>45758</v>
       </c>
-      <c r="F45" s="76">
+      <c r="F45" s="61">
         <v>45758</v>
       </c>
       <c r="G45" s="17"/>
@@ -8219,7 +8097,7 @@
       <c r="CP45" s="37"/>
       <c r="CQ45" s="40"/>
       <c r="CR45" s="37"/>
-      <c r="CS45" s="78"/>
+      <c r="CS45" s="63"/>
       <c r="CT45" s="37"/>
       <c r="CU45" s="37"/>
       <c r="CV45" s="37"/>
@@ -8246,20 +8124,20 @@
     </row>
     <row r="46" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="13"/>
-      <c r="B46" s="96" t="s">
+      <c r="B46" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="97" t="s">
+      <c r="C46" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="98">
+      <c r="D46" s="82">
         <v>0</v>
       </c>
-      <c r="E46" s="99">
+      <c r="E46" s="83">
         <f>F44</f>
         <v>45758</v>
       </c>
-      <c r="F46" s="99">
+      <c r="F46" s="83">
         <f>E46+7</f>
         <v>45765</v>
       </c>
@@ -8353,14 +8231,14 @@
       <c r="CP46" s="37"/>
       <c r="CQ46" s="40"/>
       <c r="CR46" s="37"/>
-      <c r="CS46" s="100"/>
-      <c r="CT46" s="100"/>
-      <c r="CU46" s="100"/>
-      <c r="CV46" s="100"/>
-      <c r="CW46" s="100"/>
-      <c r="CX46" s="100"/>
-      <c r="CY46" s="100"/>
-      <c r="CZ46" s="100"/>
+      <c r="CS46" s="84"/>
+      <c r="CT46" s="84"/>
+      <c r="CU46" s="84"/>
+      <c r="CV46" s="84"/>
+      <c r="CW46" s="84"/>
+      <c r="CX46" s="84"/>
+      <c r="CY46" s="84"/>
+      <c r="CZ46" s="84"/>
       <c r="DA46" s="37"/>
       <c r="DB46" s="37"/>
       <c r="DC46" s="37"/>
@@ -8380,20 +8258,20 @@
     </row>
     <row r="47" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="13"/>
-      <c r="B47" s="101" t="s">
+      <c r="B47" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="102" t="s">
+      <c r="C47" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="103">
+      <c r="D47" s="87">
         <v>0</v>
       </c>
-      <c r="E47" s="104">
+      <c r="E47" s="88">
         <f>F46</f>
         <v>45765</v>
       </c>
-      <c r="F47" s="104">
+      <c r="F47" s="88">
         <f>E47+7</f>
         <v>45772</v>
       </c>
@@ -8494,14 +8372,14 @@
       <c r="CW47" s="37"/>
       <c r="CX47" s="37"/>
       <c r="CY47" s="37"/>
-      <c r="CZ47" s="108"/>
-      <c r="DA47" s="108"/>
-      <c r="DB47" s="108"/>
-      <c r="DC47" s="108"/>
-      <c r="DD47" s="108"/>
-      <c r="DE47" s="108"/>
-      <c r="DF47" s="108"/>
-      <c r="DG47" s="108"/>
+      <c r="CZ47" s="91"/>
+      <c r="DA47" s="91"/>
+      <c r="DB47" s="91"/>
+      <c r="DC47" s="91"/>
+      <c r="DD47" s="91"/>
+      <c r="DE47" s="91"/>
+      <c r="DF47" s="91"/>
+      <c r="DG47" s="91"/>
       <c r="DH47" s="37"/>
       <c r="DI47" s="37"/>
       <c r="DJ47" s="37"/>
@@ -8514,19 +8392,19 @@
     </row>
     <row r="48" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="13"/>
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="74" t="s">
+      <c r="C48" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="75">
+      <c r="D48" s="60">
         <v>0</v>
       </c>
-      <c r="E48" s="76">
+      <c r="E48" s="61">
         <v>45775</v>
       </c>
-      <c r="F48" s="76">
+      <c r="F48" s="61">
         <v>45775</v>
       </c>
       <c r="G48" s="17"/>
@@ -8636,7 +8514,7 @@
       <c r="DG48" s="37"/>
       <c r="DH48" s="37"/>
       <c r="DI48" s="37"/>
-      <c r="DJ48" s="78"/>
+      <c r="DJ48" s="63"/>
       <c r="DK48" s="37"/>
       <c r="DL48" s="40"/>
       <c r="DM48" s="37"/>
@@ -8646,10 +8524,10 @@
     </row>
     <row r="49" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="13"/>
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="72" t="s">
+      <c r="C49" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D49" s="38">
@@ -8780,19 +8658,19 @@
     </row>
     <row r="50" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="13"/>
-      <c r="B50" s="73" t="s">
+      <c r="B50" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="75">
+      <c r="D50" s="60">
         <v>0</v>
       </c>
-      <c r="E50" s="76">
+      <c r="E50" s="61">
         <v>45779</v>
       </c>
-      <c r="F50" s="76">
+      <c r="F50" s="61">
         <v>45779</v>
       </c>
       <c r="G50" s="17"/>
@@ -8808,7 +8686,7 @@
       <c r="N50" s="37"/>
       <c r="O50" s="37"/>
       <c r="P50" s="37"/>
-      <c r="Q50" s="70"/>
+      <c r="Q50" s="37"/>
       <c r="R50" s="37"/>
       <c r="S50" s="37"/>
       <c r="T50" s="37"/>
@@ -8909,7 +8787,7 @@
       <c r="DK50" s="37"/>
       <c r="DL50" s="37"/>
       <c r="DM50" s="37"/>
-      <c r="DN50" s="78"/>
+      <c r="DN50" s="63"/>
       <c r="DO50" s="37"/>
       <c r="DP50" s="37"/>
     </row>
@@ -8918,7 +8796,7 @@
       <c r="B51" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="67"/>
+      <c r="C51" s="53"/>
       <c r="D51" s="42"/>
       <c r="E51" s="43"/>
       <c r="F51" s="44"/>
@@ -8983,6 +8861,62 @@
       <c r="BJ51" s="45"/>
       <c r="BK51" s="45"/>
       <c r="BL51" s="45"/>
+      <c r="BM51" s="45"/>
+      <c r="BN51" s="45"/>
+      <c r="BO51" s="45"/>
+      <c r="BP51" s="45"/>
+      <c r="BQ51" s="45"/>
+      <c r="BR51" s="45"/>
+      <c r="BS51" s="45"/>
+      <c r="BT51" s="45"/>
+      <c r="BU51" s="45"/>
+      <c r="BV51" s="45"/>
+      <c r="BW51" s="45"/>
+      <c r="BX51" s="45"/>
+      <c r="BY51" s="45"/>
+      <c r="BZ51" s="45"/>
+      <c r="CA51" s="45"/>
+      <c r="CB51" s="45"/>
+      <c r="CC51" s="45"/>
+      <c r="CD51" s="45"/>
+      <c r="CE51" s="45"/>
+      <c r="CF51" s="45"/>
+      <c r="CG51" s="45"/>
+      <c r="CH51" s="45"/>
+      <c r="CI51" s="45"/>
+      <c r="CJ51" s="45"/>
+      <c r="CK51" s="45"/>
+      <c r="CL51" s="45"/>
+      <c r="CM51" s="45"/>
+      <c r="CN51" s="45"/>
+      <c r="CO51" s="45"/>
+      <c r="CP51" s="45"/>
+      <c r="CQ51" s="45"/>
+      <c r="CR51" s="45"/>
+      <c r="CS51" s="45"/>
+      <c r="CT51" s="45"/>
+      <c r="CU51" s="45"/>
+      <c r="CV51" s="45"/>
+      <c r="CW51" s="45"/>
+      <c r="CX51" s="45"/>
+      <c r="CY51" s="45"/>
+      <c r="CZ51" s="45"/>
+      <c r="DA51" s="45"/>
+      <c r="DB51" s="45"/>
+      <c r="DC51" s="45"/>
+      <c r="DD51" s="45"/>
+      <c r="DE51" s="45"/>
+      <c r="DF51" s="45"/>
+      <c r="DG51" s="45"/>
+      <c r="DH51" s="45"/>
+      <c r="DI51" s="45"/>
+      <c r="DJ51" s="45"/>
+      <c r="DK51" s="45"/>
+      <c r="DL51" s="45"/>
+      <c r="DM51" s="45"/>
+      <c r="DN51" s="45"/>
+      <c r="DO51" s="45"/>
+      <c r="DP51" s="45"/>
     </row>
     <row r="52" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G52" s="3"/>
@@ -9038,110 +8972,92 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL8 I11:BL11 I10:O10 I9:L9 N9:DP9 I12:Z13 AB12:BL12 I19:BL19 I18:AN18 I26:BB26 U10:DP10 AI13:BL14 I14:AG17 I20:AN21 AW20:BL22 I27:BL27 AP15:BL18 I22:AU25 BD23:BL26 I32:BL50 I28:BB29 BK28:BL29 I30:BI31 BM41:BZ42 CB41:CD42">
-    <cfRule type="expression" dxfId="29" priority="28">
+  <conditionalFormatting sqref="I9:L9 N9:DP9 I4:BL8 I10:O10 U10:DP10 I11:BL11 AB12:BL12 I12:Z13 AI13:BL14 I14:AG17 AP15:BL18 I18:AN18 I19:BL19 I20:AN21 AW20:BL22 I22:AU25 BD23:BL26 I26:BB26 I27:BL27 I28:BB29 BK28:BL29 I30:BI31 I32:BL50 BM41:BZ42 CB41:CD42">
+    <cfRule type="expression" dxfId="21" priority="28">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:BL11 I10:O10 I12:Z13 AB12:BL12 I19:BL19 I18:AN18 I27:BL27 I26:BB26 U10:DP10 AI13:BL14 I14:AG17 I20:AN21 AW20:BL22 AP15:BL18 I22:AU25 BD23:BL26 I32:BL50 I28:BB29 BK28:BL29 I30:BI31 BM41:BZ42 CB41:CD42">
-    <cfRule type="expression" dxfId="28" priority="33">
+  <conditionalFormatting sqref="I9:L9 N9:DP9">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="8" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM4:DP4">
-    <cfRule type="expression" dxfId="26" priority="27">
+  <conditionalFormatting sqref="I10:O10 U10:DP10 I11:BL11 AB12:BL12 I12:Z13 AI13:BL14 I14:AG17 AP15:BL18 I18:AN18 I19:BL19 I20:AN21 AW20:BL22 I22:AU25 BD23:BL26 I26:BB26 I27:BL27 I28:BB29 BK28:BL29 I30:BI31 I32:BL50 BM41:BZ42 CB41:CD42">
+    <cfRule type="expression" dxfId="18" priority="34" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:BL50 I10:O10 U10:DP10 I11:BL11 AB12:BL12 I12:Z13 AI13:BL14 I14:AG17 AP15:BL18 I18:AN18 I19:BL19 I20:AN21 AW20:BL22 I22:AU25 BD23:BL26 I26:BB26 I27:BL27 I28:BB29 BK28:BL29 I30:BI31 BM41:BZ42 CB41:CD42">
+    <cfRule type="expression" dxfId="17" priority="33">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q50">
+    <cfRule type="beginsWith" dxfId="16" priority="12" operator="beginsWith" text="Milestone">
+      <formula>LEFT(Q50,LEN("Milestone"))="Milestone"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM11:CG29 BR30:CG31 BM32:CG33 BM34:BP35 BY34:CG35 BM36:CG36 BY37:CG38 BM37:BW40 CF39:CG41 BM43:CG50">
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="24" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM4:DP6">
+    <cfRule type="expression" dxfId="12" priority="25">
       <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:DP5">
-    <cfRule type="expression" dxfId="25" priority="26">
-      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
+  <conditionalFormatting sqref="BX38">
+    <cfRule type="expression" dxfId="11" priority="4">
+      <formula>AND(TODAY()&gt;=BX$5, TODAY()&lt;BY$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="5">
+      <formula>AND(task_start&lt;=BX$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BX$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BX$5,task_start&lt;BY$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM6:DP6">
-    <cfRule type="expression" dxfId="24" priority="25">
-      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM11:CG29 BM37:BW40 BM43:CG50 BM32:CG33 BR30:CG31 BM36:CG36 BM34:BP35 BY34:CG35 BY37:CG38 CF39:CG41">
-    <cfRule type="expression" dxfId="23" priority="22">
-      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM11:CG29 BM37:BW40 BM43:CG50 BM32:CG33 BR30:CG31 BM36:CG36 BM34:BP35 BY34:CG35 BY37:CG38 CF39:CG41">
-    <cfRule type="expression" dxfId="22" priority="23">
-      <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH11:CU41 CH47:CU50 CH43:CU43 CM42:CU42 CH44:CK44 CT44:CU45 CH45:CR46">
-    <cfRule type="expression" dxfId="20" priority="19">
+  <conditionalFormatting sqref="CH11:CU41 CM42:CU42 CH43:CU43 CH44:CK44 CT44:CU45 CH45:CR46 CH47:CU50">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>AND(TODAY()&gt;=CH$5, TODAY()&lt;CI$5)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH11:CU41 CH47:CU50 CH43:CU43 CM42:CU42 CH44:CK44 CT44:CU45 CH45:CR46">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="21" stopIfTrue="1">
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV11:DI45 CV48:DI50 DA46:DI46 CV47:CY47 DH47:DI47">
-    <cfRule type="expression" dxfId="17" priority="16">
+  <conditionalFormatting sqref="CV11:DI45 DA46:DI46 CV47:CY47 DH47:DI47 CV48:DI50">
+    <cfRule type="expression" dxfId="5" priority="16">
       <formula>AND(TODAY()&gt;=CV$5, TODAY()&lt;CW$5)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV11:DI45 CV48:DI50 DA46:DI46 CV47:CY47 DH47:DI47">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="4" priority="17">
       <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="18" stopIfTrue="1">
       <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DJ11:DP47 DJ49:DP49 DK48:DP48 DJ50:DM50 DO50:DP50">
-    <cfRule type="expression" dxfId="14" priority="13">
+  <conditionalFormatting sqref="DJ11:DP47 DK48:DP48 DJ49:DP49 DJ50:DM50 DO50:DP50">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>AND(TODAY()&gt;=DJ$5, TODAY()&lt;DK$5)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DJ11:DP47 DJ49:DP49 DK48:DP48 DJ50:DM50 DO50:DP50">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>AND(task_start&lt;=DJ$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DJ$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="15" stopIfTrue="1">
       <formula>AND(task_end&gt;=DJ$5,task_start&lt;DK$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q50">
-    <cfRule type="beginsWith" dxfId="11" priority="12" operator="beginsWith" text="Milestone">
-      <formula>LEFT(Q50,LEN("Milestone"))="Milestone"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9:L9 N9:DP9">
-    <cfRule type="expression" dxfId="10" priority="7">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BX38">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>AND(TODAY()&gt;=BX$5, TODAY()&lt;BY$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BX38">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>AND(task_start&lt;=BX$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BX$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BX$5,task_start&lt;BY$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="10">
@@ -9160,7 +9076,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="32" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -9236,7 +9152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="54" x14ac:dyDescent="0.35">
       <c r="A9" s="49" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
feat: update timeline from brief 3
</commit_message>
<xml_diff>
--- a/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
+++ b/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Documents\chadv1.0\chadv1.0\deliverables\timeline_and_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF40E168-FA11-4ADA-9C64-EBF8F2ACC8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F40A81-D5F7-4863-87FB-91464317A417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1061,22 +1061,19 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1091,14 +1088,17 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1894,8 +1894,8 @@
   </sheetPr>
   <dimension ref="A1:DP54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1914,60 +1914,60 @@
     <row r="1" spans="1:120" ht="90" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="100">
+      <c r="Q1" s="99">
         <f>DATE(2025, 1, 17)</f>
         <v>45674</v>
       </c>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
     </row>
     <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="I2" s="101" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="I2" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="98">
+      <c r="Q2" s="97">
         <v>1</v>
       </c>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="99"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
     </row>
     <row r="3" spans="1:120" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
@@ -1981,182 +1981,182 @@
       <c r="A4" s="14"/>
       <c r="B4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="106">
+      <c r="I4" s="94">
         <f>I5</f>
         <v>45670</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104">
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92">
         <f>P5</f>
         <v>45677</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="104"/>
-      <c r="W4" s="104">
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="92">
         <f>W5</f>
         <v>45684</v>
       </c>
-      <c r="X4" s="104"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="104"/>
-      <c r="AC4" s="104"/>
-      <c r="AD4" s="104">
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="92">
         <f>AD5</f>
         <v>45691</v>
       </c>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="104"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="104"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="104"/>
-      <c r="AK4" s="104">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="92">
         <f>AK5</f>
         <v>45698</v>
       </c>
-      <c r="AL4" s="104"/>
-      <c r="AM4" s="104"/>
-      <c r="AN4" s="104"/>
-      <c r="AO4" s="104"/>
-      <c r="AP4" s="104"/>
-      <c r="AQ4" s="104"/>
-      <c r="AR4" s="104">
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="92">
         <f>AR5</f>
         <v>45705</v>
       </c>
-      <c r="AS4" s="104"/>
-      <c r="AT4" s="104"/>
-      <c r="AU4" s="104"/>
-      <c r="AV4" s="104"/>
-      <c r="AW4" s="104"/>
-      <c r="AX4" s="104"/>
-      <c r="AY4" s="104">
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="92">
         <f>AY5</f>
         <v>45712</v>
       </c>
-      <c r="AZ4" s="104"/>
-      <c r="BA4" s="104"/>
-      <c r="BB4" s="104"/>
-      <c r="BC4" s="104"/>
-      <c r="BD4" s="104"/>
-      <c r="BE4" s="104"/>
-      <c r="BF4" s="104">
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="92">
         <f>BF5</f>
         <v>45719</v>
       </c>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="105"/>
-      <c r="BM4" s="104">
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="92">
         <f>BM5</f>
         <v>45726</v>
       </c>
-      <c r="BN4" s="104"/>
-      <c r="BO4" s="104"/>
-      <c r="BP4" s="104"/>
-      <c r="BQ4" s="104"/>
-      <c r="BR4" s="104"/>
-      <c r="BS4" s="105"/>
-      <c r="BT4" s="104">
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="92"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="92">
         <f>BT5</f>
         <v>45733</v>
       </c>
-      <c r="BU4" s="104"/>
-      <c r="BV4" s="104"/>
-      <c r="BW4" s="104"/>
-      <c r="BX4" s="104"/>
-      <c r="BY4" s="104"/>
-      <c r="BZ4" s="105"/>
-      <c r="CA4" s="104">
+      <c r="BU4" s="92"/>
+      <c r="BV4" s="92"/>
+      <c r="BW4" s="92"/>
+      <c r="BX4" s="92"/>
+      <c r="BY4" s="92"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="92">
         <f>CA5</f>
         <v>45740</v>
       </c>
-      <c r="CB4" s="104"/>
-      <c r="CC4" s="104"/>
-      <c r="CD4" s="104"/>
-      <c r="CE4" s="104"/>
-      <c r="CF4" s="104"/>
-      <c r="CG4" s="105"/>
-      <c r="CH4" s="104">
+      <c r="CB4" s="92"/>
+      <c r="CC4" s="92"/>
+      <c r="CD4" s="92"/>
+      <c r="CE4" s="92"/>
+      <c r="CF4" s="92"/>
+      <c r="CG4" s="93"/>
+      <c r="CH4" s="92">
         <f>CH5</f>
         <v>45747</v>
       </c>
-      <c r="CI4" s="104"/>
-      <c r="CJ4" s="104"/>
-      <c r="CK4" s="104"/>
-      <c r="CL4" s="104"/>
-      <c r="CM4" s="104"/>
-      <c r="CN4" s="105"/>
-      <c r="CO4" s="104">
+      <c r="CI4" s="92"/>
+      <c r="CJ4" s="92"/>
+      <c r="CK4" s="92"/>
+      <c r="CL4" s="92"/>
+      <c r="CM4" s="92"/>
+      <c r="CN4" s="93"/>
+      <c r="CO4" s="92">
         <f>CO5</f>
         <v>45754</v>
       </c>
-      <c r="CP4" s="104"/>
-      <c r="CQ4" s="104"/>
-      <c r="CR4" s="104"/>
-      <c r="CS4" s="104"/>
-      <c r="CT4" s="104"/>
-      <c r="CU4" s="105"/>
-      <c r="CV4" s="104">
+      <c r="CP4" s="92"/>
+      <c r="CQ4" s="92"/>
+      <c r="CR4" s="92"/>
+      <c r="CS4" s="92"/>
+      <c r="CT4" s="92"/>
+      <c r="CU4" s="93"/>
+      <c r="CV4" s="92">
         <f>CV5</f>
         <v>45761</v>
       </c>
-      <c r="CW4" s="104"/>
-      <c r="CX4" s="104"/>
-      <c r="CY4" s="104"/>
-      <c r="CZ4" s="104"/>
-      <c r="DA4" s="104"/>
-      <c r="DB4" s="105"/>
-      <c r="DC4" s="104">
+      <c r="CW4" s="92"/>
+      <c r="CX4" s="92"/>
+      <c r="CY4" s="92"/>
+      <c r="CZ4" s="92"/>
+      <c r="DA4" s="92"/>
+      <c r="DB4" s="93"/>
+      <c r="DC4" s="92">
         <f>DC5</f>
         <v>45768</v>
       </c>
-      <c r="DD4" s="104"/>
-      <c r="DE4" s="104"/>
-      <c r="DF4" s="104"/>
-      <c r="DG4" s="104"/>
-      <c r="DH4" s="104"/>
-      <c r="DI4" s="105"/>
-      <c r="DJ4" s="104">
+      <c r="DD4" s="92"/>
+      <c r="DE4" s="92"/>
+      <c r="DF4" s="92"/>
+      <c r="DG4" s="92"/>
+      <c r="DH4" s="92"/>
+      <c r="DI4" s="93"/>
+      <c r="DJ4" s="92">
         <f>DJ5</f>
         <v>45775</v>
       </c>
-      <c r="DK4" s="104"/>
-      <c r="DL4" s="104"/>
-      <c r="DM4" s="104"/>
-      <c r="DN4" s="104"/>
-      <c r="DO4" s="104"/>
-      <c r="DP4" s="105"/>
+      <c r="DK4" s="92"/>
+      <c r="DL4" s="92"/>
+      <c r="DM4" s="92"/>
+      <c r="DN4" s="92"/>
+      <c r="DO4" s="92"/>
+      <c r="DP4" s="93"/>
     </row>
     <row r="5" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93" t="s">
+      <c r="A5" s="103"/>
+      <c r="B5" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="95" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="24">
@@ -2609,8 +2609,8 @@
       </c>
     </row>
     <row r="6" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="92"/>
-      <c r="B6" s="94"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="96"/>
       <c r="D6" s="96"/>
       <c r="E6" s="96"/>
@@ -3886,7 +3886,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="61">
         <v>45695</v>
@@ -3921,7 +3921,7 @@
       <c r="AE14" s="37"/>
       <c r="AF14" s="37"/>
       <c r="AG14" s="37"/>
-      <c r="AH14" s="63"/>
+      <c r="AH14" s="62"/>
       <c r="AI14" s="37"/>
       <c r="AJ14" s="37"/>
       <c r="AK14" s="37"/>
@@ -8930,6 +8930,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
@@ -8938,25 +8957,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D51">
     <cfRule type="dataBar" priority="50">
@@ -9229,12 +9229,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9550,29 +9561,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9599,20 +9610,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: updated timeline to current date
</commit_message>
<xml_diff>
--- a/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
+++ b/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Documents\chadv1.0\chadv1.0\deliverables\timeline_and_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F40A81-D5F7-4863-87FB-91464317A417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A27575-BAFF-4795-8E59-501F7941FE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1061,19 +1061,22 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1088,17 +1091,14 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1894,8 +1894,8 @@
   </sheetPr>
   <dimension ref="A1:DP54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1914,60 +1914,60 @@
     <row r="1" spans="1:120" ht="90" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="99">
+      <c r="Q1" s="100">
         <f>DATE(2025, 1, 17)</f>
         <v>45674</v>
       </c>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
-      <c r="X1" s="98"/>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="98"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
     </row>
     <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="I2" s="100" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="I2" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="97">
+      <c r="Q2" s="98">
         <v>1</v>
       </c>
-      <c r="R2" s="98"/>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="98"/>
-      <c r="Z2" s="98"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
     </row>
     <row r="3" spans="1:120" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
@@ -1981,182 +1981,182 @@
       <c r="A4" s="14"/>
       <c r="B4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="94">
+      <c r="I4" s="106">
         <f>I5</f>
         <v>45670</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92">
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="104">
         <f>P5</f>
         <v>45677</v>
       </c>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92">
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="104"/>
+      <c r="W4" s="104">
         <f>W5</f>
         <v>45684</v>
       </c>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
-      <c r="Z4" s="92"/>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="92"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="92">
+      <c r="X4" s="104"/>
+      <c r="Y4" s="104"/>
+      <c r="Z4" s="104"/>
+      <c r="AA4" s="104"/>
+      <c r="AB4" s="104"/>
+      <c r="AC4" s="104"/>
+      <c r="AD4" s="104">
         <f>AD5</f>
         <v>45691</v>
       </c>
-      <c r="AE4" s="92"/>
-      <c r="AF4" s="92"/>
-      <c r="AG4" s="92"/>
-      <c r="AH4" s="92"/>
-      <c r="AI4" s="92"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="92">
+      <c r="AE4" s="104"/>
+      <c r="AF4" s="104"/>
+      <c r="AG4" s="104"/>
+      <c r="AH4" s="104"/>
+      <c r="AI4" s="104"/>
+      <c r="AJ4" s="104"/>
+      <c r="AK4" s="104">
         <f>AK5</f>
         <v>45698</v>
       </c>
-      <c r="AL4" s="92"/>
-      <c r="AM4" s="92"/>
-      <c r="AN4" s="92"/>
-      <c r="AO4" s="92"/>
-      <c r="AP4" s="92"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="92">
+      <c r="AL4" s="104"/>
+      <c r="AM4" s="104"/>
+      <c r="AN4" s="104"/>
+      <c r="AO4" s="104"/>
+      <c r="AP4" s="104"/>
+      <c r="AQ4" s="104"/>
+      <c r="AR4" s="104">
         <f>AR5</f>
         <v>45705</v>
       </c>
-      <c r="AS4" s="92"/>
-      <c r="AT4" s="92"/>
-      <c r="AU4" s="92"/>
-      <c r="AV4" s="92"/>
-      <c r="AW4" s="92"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="92">
+      <c r="AS4" s="104"/>
+      <c r="AT4" s="104"/>
+      <c r="AU4" s="104"/>
+      <c r="AV4" s="104"/>
+      <c r="AW4" s="104"/>
+      <c r="AX4" s="104"/>
+      <c r="AY4" s="104">
         <f>AY5</f>
         <v>45712</v>
       </c>
-      <c r="AZ4" s="92"/>
-      <c r="BA4" s="92"/>
-      <c r="BB4" s="92"/>
-      <c r="BC4" s="92"/>
-      <c r="BD4" s="92"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="92">
+      <c r="AZ4" s="104"/>
+      <c r="BA4" s="104"/>
+      <c r="BB4" s="104"/>
+      <c r="BC4" s="104"/>
+      <c r="BD4" s="104"/>
+      <c r="BE4" s="104"/>
+      <c r="BF4" s="104">
         <f>BF5</f>
         <v>45719</v>
       </c>
-      <c r="BG4" s="92"/>
-      <c r="BH4" s="92"/>
-      <c r="BI4" s="92"/>
-      <c r="BJ4" s="92"/>
-      <c r="BK4" s="92"/>
-      <c r="BL4" s="93"/>
-      <c r="BM4" s="92">
+      <c r="BG4" s="104"/>
+      <c r="BH4" s="104"/>
+      <c r="BI4" s="104"/>
+      <c r="BJ4" s="104"/>
+      <c r="BK4" s="104"/>
+      <c r="BL4" s="105"/>
+      <c r="BM4" s="104">
         <f>BM5</f>
         <v>45726</v>
       </c>
-      <c r="BN4" s="92"/>
-      <c r="BO4" s="92"/>
-      <c r="BP4" s="92"/>
-      <c r="BQ4" s="92"/>
-      <c r="BR4" s="92"/>
-      <c r="BS4" s="93"/>
-      <c r="BT4" s="92">
+      <c r="BN4" s="104"/>
+      <c r="BO4" s="104"/>
+      <c r="BP4" s="104"/>
+      <c r="BQ4" s="104"/>
+      <c r="BR4" s="104"/>
+      <c r="BS4" s="105"/>
+      <c r="BT4" s="104">
         <f>BT5</f>
         <v>45733</v>
       </c>
-      <c r="BU4" s="92"/>
-      <c r="BV4" s="92"/>
-      <c r="BW4" s="92"/>
-      <c r="BX4" s="92"/>
-      <c r="BY4" s="92"/>
-      <c r="BZ4" s="93"/>
-      <c r="CA4" s="92">
+      <c r="BU4" s="104"/>
+      <c r="BV4" s="104"/>
+      <c r="BW4" s="104"/>
+      <c r="BX4" s="104"/>
+      <c r="BY4" s="104"/>
+      <c r="BZ4" s="105"/>
+      <c r="CA4" s="104">
         <f>CA5</f>
         <v>45740</v>
       </c>
-      <c r="CB4" s="92"/>
-      <c r="CC4" s="92"/>
-      <c r="CD4" s="92"/>
-      <c r="CE4" s="92"/>
-      <c r="CF4" s="92"/>
-      <c r="CG4" s="93"/>
-      <c r="CH4" s="92">
+      <c r="CB4" s="104"/>
+      <c r="CC4" s="104"/>
+      <c r="CD4" s="104"/>
+      <c r="CE4" s="104"/>
+      <c r="CF4" s="104"/>
+      <c r="CG4" s="105"/>
+      <c r="CH4" s="104">
         <f>CH5</f>
         <v>45747</v>
       </c>
-      <c r="CI4" s="92"/>
-      <c r="CJ4" s="92"/>
-      <c r="CK4" s="92"/>
-      <c r="CL4" s="92"/>
-      <c r="CM4" s="92"/>
-      <c r="CN4" s="93"/>
-      <c r="CO4" s="92">
+      <c r="CI4" s="104"/>
+      <c r="CJ4" s="104"/>
+      <c r="CK4" s="104"/>
+      <c r="CL4" s="104"/>
+      <c r="CM4" s="104"/>
+      <c r="CN4" s="105"/>
+      <c r="CO4" s="104">
         <f>CO5</f>
         <v>45754</v>
       </c>
-      <c r="CP4" s="92"/>
-      <c r="CQ4" s="92"/>
-      <c r="CR4" s="92"/>
-      <c r="CS4" s="92"/>
-      <c r="CT4" s="92"/>
-      <c r="CU4" s="93"/>
-      <c r="CV4" s="92">
+      <c r="CP4" s="104"/>
+      <c r="CQ4" s="104"/>
+      <c r="CR4" s="104"/>
+      <c r="CS4" s="104"/>
+      <c r="CT4" s="104"/>
+      <c r="CU4" s="105"/>
+      <c r="CV4" s="104">
         <f>CV5</f>
         <v>45761</v>
       </c>
-      <c r="CW4" s="92"/>
-      <c r="CX4" s="92"/>
-      <c r="CY4" s="92"/>
-      <c r="CZ4" s="92"/>
-      <c r="DA4" s="92"/>
-      <c r="DB4" s="93"/>
-      <c r="DC4" s="92">
+      <c r="CW4" s="104"/>
+      <c r="CX4" s="104"/>
+      <c r="CY4" s="104"/>
+      <c r="CZ4" s="104"/>
+      <c r="DA4" s="104"/>
+      <c r="DB4" s="105"/>
+      <c r="DC4" s="104">
         <f>DC5</f>
         <v>45768</v>
       </c>
-      <c r="DD4" s="92"/>
-      <c r="DE4" s="92"/>
-      <c r="DF4" s="92"/>
-      <c r="DG4" s="92"/>
-      <c r="DH4" s="92"/>
-      <c r="DI4" s="93"/>
-      <c r="DJ4" s="92">
+      <c r="DD4" s="104"/>
+      <c r="DE4" s="104"/>
+      <c r="DF4" s="104"/>
+      <c r="DG4" s="104"/>
+      <c r="DH4" s="104"/>
+      <c r="DI4" s="105"/>
+      <c r="DJ4" s="104">
         <f>DJ5</f>
         <v>45775</v>
       </c>
-      <c r="DK4" s="92"/>
-      <c r="DL4" s="92"/>
-      <c r="DM4" s="92"/>
-      <c r="DN4" s="92"/>
-      <c r="DO4" s="92"/>
-      <c r="DP4" s="93"/>
+      <c r="DK4" s="104"/>
+      <c r="DL4" s="104"/>
+      <c r="DM4" s="104"/>
+      <c r="DN4" s="104"/>
+      <c r="DO4" s="104"/>
+      <c r="DP4" s="105"/>
     </row>
     <row r="5" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104" t="s">
+      <c r="A5" s="92"/>
+      <c r="B5" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="97" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="24">
@@ -2609,8 +2609,8 @@
       </c>
     </row>
     <row r="6" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="103"/>
-      <c r="B6" s="105"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="96"/>
       <c r="D6" s="96"/>
       <c r="E6" s="96"/>
@@ -8930,17 +8930,14 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -8949,14 +8946,17 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D51">
     <cfRule type="dataBar" priority="50">
@@ -9229,23 +9229,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9561,29 +9550,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9610,9 +9599,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: update timeline to current status
</commit_message>
<xml_diff>
--- a/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
+++ b/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Documents\chadv1.0\chadv1.0\deliverables\timeline_and_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A27575-BAFF-4795-8E59-501F7941FE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97203CF-FE19-4BD7-8990-2815D39FF2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,12 +562,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,23 +1054,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1091,15 +1081,19 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1894,8 +1888,8 @@
   </sheetPr>
   <dimension ref="A1:DP54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="54" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:DP51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1914,60 +1908,60 @@
     <row r="1" spans="1:120" ht="90" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="100">
+      <c r="Q1" s="98">
         <f>DATE(2025, 1, 17)</f>
         <v>45674</v>
       </c>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
     </row>
     <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="I2" s="101" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="I2" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="98">
+      <c r="Q2" s="96">
         <v>1</v>
       </c>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="99"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
     </row>
     <row r="3" spans="1:120" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
@@ -1981,182 +1975,182 @@
       <c r="A4" s="14"/>
       <c r="B4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="106">
+      <c r="I4" s="93">
         <f>I5</f>
         <v>45670</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91">
         <f>P5</f>
         <v>45677</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="104"/>
-      <c r="W4" s="104">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91">
         <f>W5</f>
         <v>45684</v>
       </c>
-      <c r="X4" s="104"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="104"/>
-      <c r="AC4" s="104"/>
-      <c r="AD4" s="104">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
         <v>45691</v>
       </c>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="104"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="104"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="104"/>
-      <c r="AK4" s="104">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
         <v>45698</v>
       </c>
-      <c r="AL4" s="104"/>
-      <c r="AM4" s="104"/>
-      <c r="AN4" s="104"/>
-      <c r="AO4" s="104"/>
-      <c r="AP4" s="104"/>
-      <c r="AQ4" s="104"/>
-      <c r="AR4" s="104">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
         <v>45705</v>
       </c>
-      <c r="AS4" s="104"/>
-      <c r="AT4" s="104"/>
-      <c r="AU4" s="104"/>
-      <c r="AV4" s="104"/>
-      <c r="AW4" s="104"/>
-      <c r="AX4" s="104"/>
-      <c r="AY4" s="104">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
         <v>45712</v>
       </c>
-      <c r="AZ4" s="104"/>
-      <c r="BA4" s="104"/>
-      <c r="BB4" s="104"/>
-      <c r="BC4" s="104"/>
-      <c r="BD4" s="104"/>
-      <c r="BE4" s="104"/>
-      <c r="BF4" s="104">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
         <v>45719</v>
       </c>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="105"/>
-      <c r="BM4" s="104">
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
+      <c r="BM4" s="91">
         <f>BM5</f>
         <v>45726</v>
       </c>
-      <c r="BN4" s="104"/>
-      <c r="BO4" s="104"/>
-      <c r="BP4" s="104"/>
-      <c r="BQ4" s="104"/>
-      <c r="BR4" s="104"/>
-      <c r="BS4" s="105"/>
-      <c r="BT4" s="104">
+      <c r="BN4" s="91"/>
+      <c r="BO4" s="91"/>
+      <c r="BP4" s="91"/>
+      <c r="BQ4" s="91"/>
+      <c r="BR4" s="91"/>
+      <c r="BS4" s="92"/>
+      <c r="BT4" s="91">
         <f>BT5</f>
         <v>45733</v>
       </c>
-      <c r="BU4" s="104"/>
-      <c r="BV4" s="104"/>
-      <c r="BW4" s="104"/>
-      <c r="BX4" s="104"/>
-      <c r="BY4" s="104"/>
-      <c r="BZ4" s="105"/>
-      <c r="CA4" s="104">
+      <c r="BU4" s="91"/>
+      <c r="BV4" s="91"/>
+      <c r="BW4" s="91"/>
+      <c r="BX4" s="91"/>
+      <c r="BY4" s="91"/>
+      <c r="BZ4" s="92"/>
+      <c r="CA4" s="91">
         <f>CA5</f>
         <v>45740</v>
       </c>
-      <c r="CB4" s="104"/>
-      <c r="CC4" s="104"/>
-      <c r="CD4" s="104"/>
-      <c r="CE4" s="104"/>
-      <c r="CF4" s="104"/>
-      <c r="CG4" s="105"/>
-      <c r="CH4" s="104">
+      <c r="CB4" s="91"/>
+      <c r="CC4" s="91"/>
+      <c r="CD4" s="91"/>
+      <c r="CE4" s="91"/>
+      <c r="CF4" s="91"/>
+      <c r="CG4" s="92"/>
+      <c r="CH4" s="91">
         <f>CH5</f>
         <v>45747</v>
       </c>
-      <c r="CI4" s="104"/>
-      <c r="CJ4" s="104"/>
-      <c r="CK4" s="104"/>
-      <c r="CL4" s="104"/>
-      <c r="CM4" s="104"/>
-      <c r="CN4" s="105"/>
-      <c r="CO4" s="104">
+      <c r="CI4" s="91"/>
+      <c r="CJ4" s="91"/>
+      <c r="CK4" s="91"/>
+      <c r="CL4" s="91"/>
+      <c r="CM4" s="91"/>
+      <c r="CN4" s="92"/>
+      <c r="CO4" s="91">
         <f>CO5</f>
         <v>45754</v>
       </c>
-      <c r="CP4" s="104"/>
-      <c r="CQ4" s="104"/>
-      <c r="CR4" s="104"/>
-      <c r="CS4" s="104"/>
-      <c r="CT4" s="104"/>
-      <c r="CU4" s="105"/>
-      <c r="CV4" s="104">
+      <c r="CP4" s="91"/>
+      <c r="CQ4" s="91"/>
+      <c r="CR4" s="91"/>
+      <c r="CS4" s="91"/>
+      <c r="CT4" s="91"/>
+      <c r="CU4" s="92"/>
+      <c r="CV4" s="91">
         <f>CV5</f>
         <v>45761</v>
       </c>
-      <c r="CW4" s="104"/>
-      <c r="CX4" s="104"/>
-      <c r="CY4" s="104"/>
-      <c r="CZ4" s="104"/>
-      <c r="DA4" s="104"/>
-      <c r="DB4" s="105"/>
-      <c r="DC4" s="104">
+      <c r="CW4" s="91"/>
+      <c r="CX4" s="91"/>
+      <c r="CY4" s="91"/>
+      <c r="CZ4" s="91"/>
+      <c r="DA4" s="91"/>
+      <c r="DB4" s="92"/>
+      <c r="DC4" s="91">
         <f>DC5</f>
         <v>45768</v>
       </c>
-      <c r="DD4" s="104"/>
-      <c r="DE4" s="104"/>
-      <c r="DF4" s="104"/>
-      <c r="DG4" s="104"/>
-      <c r="DH4" s="104"/>
-      <c r="DI4" s="105"/>
-      <c r="DJ4" s="104">
+      <c r="DD4" s="91"/>
+      <c r="DE4" s="91"/>
+      <c r="DF4" s="91"/>
+      <c r="DG4" s="91"/>
+      <c r="DH4" s="91"/>
+      <c r="DI4" s="92"/>
+      <c r="DJ4" s="91">
         <f>DJ5</f>
         <v>45775</v>
       </c>
-      <c r="DK4" s="104"/>
-      <c r="DL4" s="104"/>
-      <c r="DM4" s="104"/>
-      <c r="DN4" s="104"/>
-      <c r="DO4" s="104"/>
-      <c r="DP4" s="105"/>
+      <c r="DK4" s="91"/>
+      <c r="DL4" s="91"/>
+      <c r="DM4" s="91"/>
+      <c r="DN4" s="91"/>
+      <c r="DO4" s="91"/>
+      <c r="DP4" s="92"/>
     </row>
     <row r="5" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="94" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="24">
@@ -2609,12 +2603,12 @@
       </c>
     </row>
     <row r="6" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="92"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
       <c r="I6" s="27" t="str">
         <f t="shared" ref="I6:AN6" si="43">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -4018,7 +4012,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="83">
         <f>F13</f>
@@ -4058,14 +4052,14 @@
       <c r="AE15" s="37"/>
       <c r="AF15" s="37"/>
       <c r="AG15" s="37"/>
-      <c r="AH15" s="84"/>
-      <c r="AI15" s="84"/>
-      <c r="AJ15" s="84"/>
-      <c r="AK15" s="84"/>
-      <c r="AL15" s="84"/>
-      <c r="AM15" s="84"/>
-      <c r="AN15" s="84"/>
-      <c r="AO15" s="84"/>
+      <c r="AH15" s="75"/>
+      <c r="AI15" s="75"/>
+      <c r="AJ15" s="75"/>
+      <c r="AK15" s="75"/>
+      <c r="AL15" s="75"/>
+      <c r="AM15" s="75"/>
+      <c r="AN15" s="75"/>
+      <c r="AO15" s="75"/>
       <c r="AP15" s="37"/>
       <c r="AQ15" s="37"/>
       <c r="AR15" s="37"/>
@@ -4155,7 +4149,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="73">
         <v>45695</v>
@@ -4190,14 +4184,14 @@
       <c r="AE16" s="37"/>
       <c r="AF16" s="37"/>
       <c r="AG16" s="37"/>
-      <c r="AH16" s="89"/>
-      <c r="AI16" s="89"/>
-      <c r="AJ16" s="89"/>
-      <c r="AK16" s="89"/>
-      <c r="AL16" s="89"/>
-      <c r="AM16" s="89"/>
-      <c r="AN16" s="89"/>
-      <c r="AO16" s="89"/>
+      <c r="AH16" s="74"/>
+      <c r="AI16" s="74"/>
+      <c r="AJ16" s="74"/>
+      <c r="AK16" s="74"/>
+      <c r="AL16" s="74"/>
+      <c r="AM16" s="74"/>
+      <c r="AN16" s="74"/>
+      <c r="AO16" s="74"/>
       <c r="AP16" s="37"/>
       <c r="AQ16" s="37"/>
       <c r="AR16" s="37"/>
@@ -4287,7 +4281,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="36">
         <v>45695</v>
@@ -4322,14 +4316,14 @@
       <c r="AE17" s="37"/>
       <c r="AF17" s="37"/>
       <c r="AG17" s="37"/>
-      <c r="AH17" s="90"/>
-      <c r="AI17" s="90"/>
-      <c r="AJ17" s="90"/>
-      <c r="AK17" s="90"/>
-      <c r="AL17" s="90"/>
-      <c r="AM17" s="90"/>
-      <c r="AN17" s="90"/>
-      <c r="AO17" s="90"/>
+      <c r="AH17" s="106"/>
+      <c r="AI17" s="106"/>
+      <c r="AJ17" s="106"/>
+      <c r="AK17" s="106"/>
+      <c r="AL17" s="106"/>
+      <c r="AM17" s="106"/>
+      <c r="AN17" s="106"/>
+      <c r="AO17" s="106"/>
       <c r="AP17" s="37"/>
       <c r="AQ17" s="37"/>
       <c r="AR17" s="37"/>
@@ -4419,7 +4413,7 @@
         <v>33</v>
       </c>
       <c r="D18" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="61">
         <v>45702</v>
@@ -4461,7 +4455,7 @@
       <c r="AL18" s="37"/>
       <c r="AM18" s="37"/>
       <c r="AN18" s="37"/>
-      <c r="AO18" s="63"/>
+      <c r="AO18" s="62"/>
       <c r="AP18" s="37"/>
       <c r="AQ18" s="37"/>
       <c r="AR18" s="37"/>
@@ -4551,7 +4545,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="39">
         <f>F15</f>
@@ -4685,7 +4679,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="79">
         <v>45702</v>
@@ -4727,14 +4721,14 @@
       <c r="AL20" s="37"/>
       <c r="AM20" s="37"/>
       <c r="AN20" s="37"/>
-      <c r="AO20" s="84"/>
-      <c r="AP20" s="84"/>
-      <c r="AQ20" s="84"/>
-      <c r="AR20" s="84"/>
-      <c r="AS20" s="84"/>
-      <c r="AT20" s="84"/>
-      <c r="AU20" s="84"/>
-      <c r="AV20" s="84"/>
+      <c r="AO20" s="75"/>
+      <c r="AP20" s="75"/>
+      <c r="AQ20" s="75"/>
+      <c r="AR20" s="75"/>
+      <c r="AS20" s="75"/>
+      <c r="AT20" s="75"/>
+      <c r="AU20" s="75"/>
+      <c r="AV20" s="75"/>
       <c r="AW20" s="37"/>
       <c r="AX20" s="37"/>
       <c r="AY20" s="37"/>
@@ -4817,7 +4811,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="73">
         <v>45702</v>
@@ -4859,14 +4853,14 @@
       <c r="AL21" s="37"/>
       <c r="AM21" s="37"/>
       <c r="AN21" s="37"/>
-      <c r="AO21" s="91"/>
-      <c r="AP21" s="91"/>
-      <c r="AQ21" s="91"/>
-      <c r="AR21" s="91"/>
-      <c r="AS21" s="91"/>
-      <c r="AT21" s="91"/>
-      <c r="AU21" s="91"/>
-      <c r="AV21" s="91"/>
+      <c r="AO21" s="74"/>
+      <c r="AP21" s="74"/>
+      <c r="AQ21" s="74"/>
+      <c r="AR21" s="74"/>
+      <c r="AS21" s="74"/>
+      <c r="AT21" s="74"/>
+      <c r="AU21" s="74"/>
+      <c r="AV21" s="74"/>
       <c r="AW21" s="37"/>
       <c r="AX21" s="37"/>
       <c r="AY21" s="37"/>
@@ -4949,7 +4943,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="61">
         <v>45709</v>
@@ -4998,7 +4992,7 @@
       <c r="AS22" s="37"/>
       <c r="AT22" s="37"/>
       <c r="AU22" s="37"/>
-      <c r="AV22" s="63"/>
+      <c r="AV22" s="62"/>
       <c r="AW22" s="37"/>
       <c r="AX22" s="37"/>
       <c r="AY22" s="37"/>
@@ -5132,14 +5126,14 @@
       <c r="AS23" s="37"/>
       <c r="AT23" s="37"/>
       <c r="AU23" s="37"/>
-      <c r="AV23" s="91"/>
-      <c r="AW23" s="91"/>
-      <c r="AX23" s="91"/>
-      <c r="AY23" s="91"/>
-      <c r="AZ23" s="91"/>
-      <c r="BA23" s="91"/>
-      <c r="BB23" s="91"/>
-      <c r="BC23" s="91"/>
+      <c r="AV23" s="90"/>
+      <c r="AW23" s="90"/>
+      <c r="AX23" s="90"/>
+      <c r="AY23" s="90"/>
+      <c r="AZ23" s="90"/>
+      <c r="BA23" s="90"/>
+      <c r="BB23" s="90"/>
+      <c r="BC23" s="90"/>
       <c r="BD23" s="37"/>
       <c r="BE23" s="37"/>
       <c r="BF23" s="37"/>
@@ -5396,14 +5390,14 @@
       <c r="AS25" s="37"/>
       <c r="AT25" s="37"/>
       <c r="AU25" s="37"/>
-      <c r="AV25" s="90"/>
-      <c r="AW25" s="90"/>
-      <c r="AX25" s="90"/>
-      <c r="AY25" s="90"/>
-      <c r="AZ25" s="90"/>
-      <c r="BA25" s="90"/>
-      <c r="BB25" s="90"/>
-      <c r="BC25" s="90"/>
+      <c r="AV25" s="89"/>
+      <c r="AW25" s="89"/>
+      <c r="AX25" s="89"/>
+      <c r="AY25" s="89"/>
+      <c r="AZ25" s="89"/>
+      <c r="BA25" s="89"/>
+      <c r="BB25" s="89"/>
+      <c r="BC25" s="89"/>
       <c r="BD25" s="37"/>
       <c r="BE25" s="37"/>
       <c r="BF25" s="37"/>
@@ -5803,14 +5797,14 @@
       <c r="AZ28" s="37"/>
       <c r="BA28" s="37"/>
       <c r="BB28" s="37"/>
-      <c r="BC28" s="91"/>
-      <c r="BD28" s="91"/>
-      <c r="BE28" s="91"/>
-      <c r="BF28" s="91"/>
-      <c r="BG28" s="91"/>
-      <c r="BH28" s="91"/>
-      <c r="BI28" s="91"/>
-      <c r="BJ28" s="91"/>
+      <c r="BC28" s="90"/>
+      <c r="BD28" s="90"/>
+      <c r="BE28" s="90"/>
+      <c r="BF28" s="90"/>
+      <c r="BG28" s="90"/>
+      <c r="BH28" s="90"/>
+      <c r="BI28" s="90"/>
+      <c r="BJ28" s="90"/>
       <c r="BK28" s="37"/>
       <c r="BL28" s="37"/>
       <c r="BM28" s="37"/>
@@ -6208,14 +6202,14 @@
       <c r="BG31" s="37"/>
       <c r="BH31" s="37"/>
       <c r="BI31" s="37"/>
-      <c r="BJ31" s="91"/>
-      <c r="BK31" s="91"/>
-      <c r="BL31" s="91"/>
-      <c r="BM31" s="91"/>
-      <c r="BN31" s="91"/>
-      <c r="BO31" s="91"/>
-      <c r="BP31" s="91"/>
-      <c r="BQ31" s="91"/>
+      <c r="BJ31" s="90"/>
+      <c r="BK31" s="90"/>
+      <c r="BL31" s="90"/>
+      <c r="BM31" s="90"/>
+      <c r="BN31" s="90"/>
+      <c r="BO31" s="90"/>
+      <c r="BP31" s="90"/>
+      <c r="BQ31" s="90"/>
       <c r="BR31" s="37"/>
       <c r="BS31" s="37"/>
       <c r="BT31" s="37"/>
@@ -6743,14 +6737,14 @@
       <c r="BN35" s="37"/>
       <c r="BO35" s="37"/>
       <c r="BP35" s="37"/>
-      <c r="BQ35" s="91"/>
-      <c r="BR35" s="91"/>
-      <c r="BS35" s="91"/>
-      <c r="BT35" s="91"/>
-      <c r="BU35" s="91"/>
-      <c r="BV35" s="91"/>
-      <c r="BW35" s="91"/>
-      <c r="BX35" s="91"/>
+      <c r="BQ35" s="90"/>
+      <c r="BR35" s="90"/>
+      <c r="BS35" s="90"/>
+      <c r="BT35" s="90"/>
+      <c r="BU35" s="90"/>
+      <c r="BV35" s="90"/>
+      <c r="BW35" s="90"/>
+      <c r="BX35" s="90"/>
       <c r="BY35" s="37"/>
       <c r="BZ35" s="37"/>
       <c r="CA35" s="37"/>
@@ -7280,14 +7274,14 @@
       <c r="BU39" s="37"/>
       <c r="BV39" s="37"/>
       <c r="BW39" s="37"/>
-      <c r="BX39" s="91"/>
-      <c r="BY39" s="91"/>
-      <c r="BZ39" s="91"/>
-      <c r="CA39" s="91"/>
-      <c r="CB39" s="91"/>
-      <c r="CC39" s="91"/>
-      <c r="CD39" s="91"/>
-      <c r="CE39" s="91"/>
+      <c r="BX39" s="90"/>
+      <c r="BY39" s="90"/>
+      <c r="BZ39" s="90"/>
+      <c r="CA39" s="90"/>
+      <c r="CB39" s="90"/>
+      <c r="CC39" s="90"/>
+      <c r="CD39" s="90"/>
+      <c r="CE39" s="90"/>
       <c r="CF39" s="37"/>
       <c r="CG39" s="37"/>
       <c r="CH39" s="37"/>
@@ -7958,14 +7952,14 @@
       <c r="CI44" s="37"/>
       <c r="CJ44" s="37"/>
       <c r="CK44" s="37"/>
-      <c r="CL44" s="91"/>
-      <c r="CM44" s="91"/>
-      <c r="CN44" s="91"/>
-      <c r="CO44" s="91"/>
-      <c r="CP44" s="91"/>
-      <c r="CQ44" s="91"/>
-      <c r="CR44" s="91"/>
-      <c r="CS44" s="91"/>
+      <c r="CL44" s="90"/>
+      <c r="CM44" s="90"/>
+      <c r="CN44" s="90"/>
+      <c r="CO44" s="90"/>
+      <c r="CP44" s="90"/>
+      <c r="CQ44" s="90"/>
+      <c r="CR44" s="90"/>
+      <c r="CS44" s="90"/>
       <c r="CT44" s="37"/>
       <c r="CU44" s="37"/>
       <c r="CV44" s="37"/>
@@ -8372,14 +8366,14 @@
       <c r="CW47" s="37"/>
       <c r="CX47" s="37"/>
       <c r="CY47" s="37"/>
-      <c r="CZ47" s="91"/>
-      <c r="DA47" s="91"/>
-      <c r="DB47" s="91"/>
-      <c r="DC47" s="91"/>
-      <c r="DD47" s="91"/>
-      <c r="DE47" s="91"/>
-      <c r="DF47" s="91"/>
-      <c r="DG47" s="91"/>
+      <c r="CZ47" s="90"/>
+      <c r="DA47" s="90"/>
+      <c r="DB47" s="90"/>
+      <c r="DC47" s="90"/>
+      <c r="DD47" s="90"/>
+      <c r="DE47" s="90"/>
+      <c r="DF47" s="90"/>
+      <c r="DG47" s="90"/>
       <c r="DH47" s="37"/>
       <c r="DI47" s="37"/>
       <c r="DJ47" s="37"/>
@@ -8930,6 +8924,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
@@ -8938,25 +8951,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D51">
     <cfRule type="dataBar" priority="50">
@@ -9152,7 +9146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A9" s="49" t="s">
         <v>16</v>
       </c>
@@ -9229,12 +9223,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9550,29 +9555,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9599,20 +9604,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: final syntax & formatting
</commit_message>
<xml_diff>
--- a/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
+++ b/deliverables/timeline_and_milestones/Project_Timeline_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Documents\chadv1.0\chadv1.0\deliverables\timeline_and_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97203CF-FE19-4BD7-8990-2815D39FF2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D83675-95C4-4283-BB80-49B08A8469E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,12 +543,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -556,24 +550,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,7 +788,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -982,20 +958,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1014,7 +989,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1039,7 +1014,6 @@
     <xf numFmtId="164" fontId="16" fillId="5" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1052,21 +1026,23 @@
     <xf numFmtId="164" fontId="16" fillId="4" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1081,19 +1057,15 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1888,8 +1860,8 @@
   </sheetPr>
   <dimension ref="A1:DP54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="54" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:DP51"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1908,64 +1880,64 @@
     <row r="1" spans="1:120" ht="90" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="98">
+      <c r="Q1" s="96">
         <f>DATE(2025, 1, 17)</f>
         <v>45674</v>
       </c>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
     </row>
     <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="I2" s="99" t="s">
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="I2" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="96">
+      <c r="Q2" s="94">
         <v>1</v>
       </c>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="95"/>
     </row>
     <row r="3" spans="1:120" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="68" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="20"/>
@@ -1975,182 +1947,182 @@
       <c r="A4" s="14"/>
       <c r="B4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="I4" s="93">
+      <c r="I4" s="102">
         <f>I5</f>
         <v>45670</v>
       </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91">
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100">
         <f>P5</f>
         <v>45677</v>
       </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91">
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="100"/>
+      <c r="W4" s="100">
         <f>W5</f>
         <v>45684</v>
       </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="91">
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AC4" s="100"/>
+      <c r="AD4" s="100">
         <f>AD5</f>
         <v>45691</v>
       </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="91">
+      <c r="AE4" s="100"/>
+      <c r="AF4" s="100"/>
+      <c r="AG4" s="100"/>
+      <c r="AH4" s="100"/>
+      <c r="AI4" s="100"/>
+      <c r="AJ4" s="100"/>
+      <c r="AK4" s="100">
         <f>AK5</f>
         <v>45698</v>
       </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="91">
+      <c r="AL4" s="100"/>
+      <c r="AM4" s="100"/>
+      <c r="AN4" s="100"/>
+      <c r="AO4" s="100"/>
+      <c r="AP4" s="100"/>
+      <c r="AQ4" s="100"/>
+      <c r="AR4" s="100">
         <f>AR5</f>
         <v>45705</v>
       </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="91">
+      <c r="AS4" s="100"/>
+      <c r="AT4" s="100"/>
+      <c r="AU4" s="100"/>
+      <c r="AV4" s="100"/>
+      <c r="AW4" s="100"/>
+      <c r="AX4" s="100"/>
+      <c r="AY4" s="100">
         <f>AY5</f>
         <v>45712</v>
       </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="91">
+      <c r="AZ4" s="100"/>
+      <c r="BA4" s="100"/>
+      <c r="BB4" s="100"/>
+      <c r="BC4" s="100"/>
+      <c r="BD4" s="100"/>
+      <c r="BE4" s="100"/>
+      <c r="BF4" s="100">
         <f>BF5</f>
         <v>45719</v>
       </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
-      <c r="BM4" s="91">
+      <c r="BG4" s="100"/>
+      <c r="BH4" s="100"/>
+      <c r="BI4" s="100"/>
+      <c r="BJ4" s="100"/>
+      <c r="BK4" s="100"/>
+      <c r="BL4" s="101"/>
+      <c r="BM4" s="100">
         <f>BM5</f>
         <v>45726</v>
       </c>
-      <c r="BN4" s="91"/>
-      <c r="BO4" s="91"/>
-      <c r="BP4" s="91"/>
-      <c r="BQ4" s="91"/>
-      <c r="BR4" s="91"/>
-      <c r="BS4" s="92"/>
-      <c r="BT4" s="91">
+      <c r="BN4" s="100"/>
+      <c r="BO4" s="100"/>
+      <c r="BP4" s="100"/>
+      <c r="BQ4" s="100"/>
+      <c r="BR4" s="100"/>
+      <c r="BS4" s="101"/>
+      <c r="BT4" s="100">
         <f>BT5</f>
         <v>45733</v>
       </c>
-      <c r="BU4" s="91"/>
-      <c r="BV4" s="91"/>
-      <c r="BW4" s="91"/>
-      <c r="BX4" s="91"/>
-      <c r="BY4" s="91"/>
-      <c r="BZ4" s="92"/>
-      <c r="CA4" s="91">
+      <c r="BU4" s="100"/>
+      <c r="BV4" s="100"/>
+      <c r="BW4" s="100"/>
+      <c r="BX4" s="100"/>
+      <c r="BY4" s="100"/>
+      <c r="BZ4" s="101"/>
+      <c r="CA4" s="100">
         <f>CA5</f>
         <v>45740</v>
       </c>
-      <c r="CB4" s="91"/>
-      <c r="CC4" s="91"/>
-      <c r="CD4" s="91"/>
-      <c r="CE4" s="91"/>
-      <c r="CF4" s="91"/>
-      <c r="CG4" s="92"/>
-      <c r="CH4" s="91">
+      <c r="CB4" s="100"/>
+      <c r="CC4" s="100"/>
+      <c r="CD4" s="100"/>
+      <c r="CE4" s="100"/>
+      <c r="CF4" s="100"/>
+      <c r="CG4" s="101"/>
+      <c r="CH4" s="100">
         <f>CH5</f>
         <v>45747</v>
       </c>
-      <c r="CI4" s="91"/>
-      <c r="CJ4" s="91"/>
-      <c r="CK4" s="91"/>
-      <c r="CL4" s="91"/>
-      <c r="CM4" s="91"/>
-      <c r="CN4" s="92"/>
-      <c r="CO4" s="91">
+      <c r="CI4" s="100"/>
+      <c r="CJ4" s="100"/>
+      <c r="CK4" s="100"/>
+      <c r="CL4" s="100"/>
+      <c r="CM4" s="100"/>
+      <c r="CN4" s="101"/>
+      <c r="CO4" s="100">
         <f>CO5</f>
         <v>45754</v>
       </c>
-      <c r="CP4" s="91"/>
-      <c r="CQ4" s="91"/>
-      <c r="CR4" s="91"/>
-      <c r="CS4" s="91"/>
-      <c r="CT4" s="91"/>
-      <c r="CU4" s="92"/>
-      <c r="CV4" s="91">
+      <c r="CP4" s="100"/>
+      <c r="CQ4" s="100"/>
+      <c r="CR4" s="100"/>
+      <c r="CS4" s="100"/>
+      <c r="CT4" s="100"/>
+      <c r="CU4" s="101"/>
+      <c r="CV4" s="100">
         <f>CV5</f>
         <v>45761</v>
       </c>
-      <c r="CW4" s="91"/>
-      <c r="CX4" s="91"/>
-      <c r="CY4" s="91"/>
-      <c r="CZ4" s="91"/>
-      <c r="DA4" s="91"/>
-      <c r="DB4" s="92"/>
-      <c r="DC4" s="91">
+      <c r="CW4" s="100"/>
+      <c r="CX4" s="100"/>
+      <c r="CY4" s="100"/>
+      <c r="CZ4" s="100"/>
+      <c r="DA4" s="100"/>
+      <c r="DB4" s="101"/>
+      <c r="DC4" s="100">
         <f>DC5</f>
         <v>45768</v>
       </c>
-      <c r="DD4" s="91"/>
-      <c r="DE4" s="91"/>
-      <c r="DF4" s="91"/>
-      <c r="DG4" s="91"/>
-      <c r="DH4" s="91"/>
-      <c r="DI4" s="92"/>
-      <c r="DJ4" s="91">
+      <c r="DD4" s="100"/>
+      <c r="DE4" s="100"/>
+      <c r="DF4" s="100"/>
+      <c r="DG4" s="100"/>
+      <c r="DH4" s="100"/>
+      <c r="DI4" s="101"/>
+      <c r="DJ4" s="100">
         <f>DJ5</f>
         <v>45775</v>
       </c>
-      <c r="DK4" s="91"/>
-      <c r="DL4" s="91"/>
-      <c r="DM4" s="91"/>
-      <c r="DN4" s="91"/>
-      <c r="DO4" s="91"/>
-      <c r="DP4" s="92"/>
+      <c r="DK4" s="100"/>
+      <c r="DL4" s="100"/>
+      <c r="DM4" s="100"/>
+      <c r="DN4" s="100"/>
+      <c r="DO4" s="100"/>
+      <c r="DP4" s="101"/>
     </row>
     <row r="5" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103" t="s">
+      <c r="A5" s="88"/>
+      <c r="B5" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="94" t="s">
+      <c r="F5" s="93" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="24">
@@ -2603,12 +2575,12 @@
       </c>
     </row>
     <row r="6" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="102"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
       <c r="I6" s="27" t="str">
         <f t="shared" ref="I6:AN6" si="43">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -3130,13 +3102,13 @@
     </row>
     <row r="8" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14"/>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="68"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
         <f t="shared" ref="H8:H51" si="51">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -3331,19 +3303,19 @@
     </row>
     <row r="10" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="71">
         <v>1</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="72">
         <v>45677</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="72">
         <f>E10+4</f>
         <v>45681</v>
       </c>
@@ -3359,11 +3331,11 @@
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="74"/>
-      <c r="T10" s="74"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
       <c r="U10" s="37"/>
       <c r="V10" s="37"/>
       <c r="W10" s="37"/>
@@ -3736,20 +3708,20 @@
     </row>
     <row r="13" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="82">
+      <c r="D13" s="81">
         <v>1</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="82">
         <f>F11</f>
         <v>45688</v>
       </c>
-      <c r="F13" s="83">
+      <c r="F13" s="82">
         <f>E13+7</f>
         <v>45695</v>
       </c>
@@ -3776,14 +3748,14 @@
       <c r="X13" s="37"/>
       <c r="Y13" s="37"/>
       <c r="Z13" s="37"/>
-      <c r="AA13" s="75"/>
-      <c r="AB13" s="75"/>
-      <c r="AC13" s="75"/>
-      <c r="AD13" s="75"/>
-      <c r="AE13" s="75"/>
-      <c r="AF13" s="75"/>
-      <c r="AG13" s="75"/>
-      <c r="AH13" s="75"/>
+      <c r="AA13" s="74"/>
+      <c r="AB13" s="74"/>
+      <c r="AC13" s="74"/>
+      <c r="AD13" s="74"/>
+      <c r="AE13" s="74"/>
+      <c r="AF13" s="74"/>
+      <c r="AG13" s="74"/>
+      <c r="AH13" s="74"/>
       <c r="AI13" s="37"/>
       <c r="AJ13" s="37"/>
       <c r="AK13" s="37"/>
@@ -4005,20 +3977,20 @@
     </row>
     <row r="15" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13"/>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="82">
+      <c r="D15" s="81">
         <v>1</v>
       </c>
-      <c r="E15" s="83">
+      <c r="E15" s="82">
         <f>F13</f>
         <v>45695</v>
       </c>
-      <c r="F15" s="83">
+      <c r="F15" s="82">
         <f>E15+7</f>
         <v>45702</v>
       </c>
@@ -4052,14 +4024,14 @@
       <c r="AE15" s="37"/>
       <c r="AF15" s="37"/>
       <c r="AG15" s="37"/>
-      <c r="AH15" s="75"/>
-      <c r="AI15" s="75"/>
-      <c r="AJ15" s="75"/>
-      <c r="AK15" s="75"/>
-      <c r="AL15" s="75"/>
-      <c r="AM15" s="75"/>
-      <c r="AN15" s="75"/>
-      <c r="AO15" s="75"/>
+      <c r="AH15" s="74"/>
+      <c r="AI15" s="74"/>
+      <c r="AJ15" s="74"/>
+      <c r="AK15" s="74"/>
+      <c r="AL15" s="74"/>
+      <c r="AM15" s="74"/>
+      <c r="AN15" s="74"/>
+      <c r="AO15" s="74"/>
       <c r="AP15" s="37"/>
       <c r="AQ15" s="37"/>
       <c r="AR15" s="37"/>
@@ -4142,19 +4114,19 @@
     </row>
     <row r="16" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="13"/>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="71">
         <v>1</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="72">
         <v>45695</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="72">
         <v>45702</v>
       </c>
       <c r="G16" s="17"/>
@@ -4184,14 +4156,14 @@
       <c r="AE16" s="37"/>
       <c r="AF16" s="37"/>
       <c r="AG16" s="37"/>
-      <c r="AH16" s="74"/>
-      <c r="AI16" s="74"/>
-      <c r="AJ16" s="74"/>
-      <c r="AK16" s="74"/>
-      <c r="AL16" s="74"/>
-      <c r="AM16" s="74"/>
-      <c r="AN16" s="74"/>
-      <c r="AO16" s="74"/>
+      <c r="AH16" s="73"/>
+      <c r="AI16" s="73"/>
+      <c r="AJ16" s="73"/>
+      <c r="AK16" s="73"/>
+      <c r="AL16" s="73"/>
+      <c r="AM16" s="73"/>
+      <c r="AN16" s="73"/>
+      <c r="AO16" s="73"/>
       <c r="AP16" s="37"/>
       <c r="AQ16" s="37"/>
       <c r="AR16" s="37"/>
@@ -4316,14 +4288,14 @@
       <c r="AE17" s="37"/>
       <c r="AF17" s="37"/>
       <c r="AG17" s="37"/>
-      <c r="AH17" s="106"/>
-      <c r="AI17" s="106"/>
-      <c r="AJ17" s="106"/>
-      <c r="AK17" s="106"/>
-      <c r="AL17" s="106"/>
-      <c r="AM17" s="106"/>
-      <c r="AN17" s="106"/>
-      <c r="AO17" s="106"/>
+      <c r="AH17" s="87"/>
+      <c r="AI17" s="87"/>
+      <c r="AJ17" s="87"/>
+      <c r="AK17" s="87"/>
+      <c r="AL17" s="87"/>
+      <c r="AM17" s="87"/>
+      <c r="AN17" s="87"/>
+      <c r="AO17" s="87"/>
       <c r="AP17" s="37"/>
       <c r="AQ17" s="37"/>
       <c r="AR17" s="37"/>
@@ -4672,19 +4644,19 @@
     </row>
     <row r="20" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13"/>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="78">
+      <c r="D20" s="77">
         <v>1</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="78">
         <v>45702</v>
       </c>
-      <c r="F20" s="79">
+      <c r="F20" s="78">
         <v>45709</v>
       </c>
       <c r="G20" s="17"/>
@@ -4721,14 +4693,14 @@
       <c r="AL20" s="37"/>
       <c r="AM20" s="37"/>
       <c r="AN20" s="37"/>
-      <c r="AO20" s="75"/>
-      <c r="AP20" s="75"/>
-      <c r="AQ20" s="75"/>
-      <c r="AR20" s="75"/>
-      <c r="AS20" s="75"/>
-      <c r="AT20" s="75"/>
-      <c r="AU20" s="75"/>
-      <c r="AV20" s="75"/>
+      <c r="AO20" s="74"/>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="74"/>
+      <c r="AR20" s="74"/>
+      <c r="AS20" s="74"/>
+      <c r="AT20" s="74"/>
+      <c r="AU20" s="74"/>
+      <c r="AV20" s="74"/>
       <c r="AW20" s="37"/>
       <c r="AX20" s="37"/>
       <c r="AY20" s="37"/>
@@ -4804,19 +4776,19 @@
     </row>
     <row r="21" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="13"/>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="71">
         <v>1</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="72">
         <v>45702</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="72">
         <v>45709</v>
       </c>
       <c r="G21" s="17"/>
@@ -4853,14 +4825,14 @@
       <c r="AL21" s="37"/>
       <c r="AM21" s="37"/>
       <c r="AN21" s="37"/>
-      <c r="AO21" s="74"/>
-      <c r="AP21" s="74"/>
-      <c r="AQ21" s="74"/>
-      <c r="AR21" s="74"/>
-      <c r="AS21" s="74"/>
-      <c r="AT21" s="74"/>
-      <c r="AU21" s="74"/>
-      <c r="AV21" s="74"/>
+      <c r="AO21" s="73"/>
+      <c r="AP21" s="73"/>
+      <c r="AQ21" s="73"/>
+      <c r="AR21" s="73"/>
+      <c r="AS21" s="73"/>
+      <c r="AT21" s="73"/>
+      <c r="AU21" s="73"/>
+      <c r="AV21" s="73"/>
       <c r="AW21" s="37"/>
       <c r="AX21" s="37"/>
       <c r="AY21" s="37"/>
@@ -5068,20 +5040,20 @@
     </row>
     <row r="23" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="13"/>
-      <c r="B23" s="85" t="s">
+      <c r="B23" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="87">
-        <v>0</v>
-      </c>
-      <c r="E23" s="88">
+      <c r="D23" s="85">
+        <v>1</v>
+      </c>
+      <c r="E23" s="86">
         <f>F19</f>
         <v>45709</v>
       </c>
-      <c r="F23" s="88">
+      <c r="F23" s="86">
         <f>E23+7</f>
         <v>45716</v>
       </c>
@@ -5126,14 +5098,14 @@
       <c r="AS23" s="37"/>
       <c r="AT23" s="37"/>
       <c r="AU23" s="37"/>
-      <c r="AV23" s="90"/>
-      <c r="AW23" s="90"/>
-      <c r="AX23" s="90"/>
-      <c r="AY23" s="90"/>
-      <c r="AZ23" s="90"/>
-      <c r="BA23" s="90"/>
-      <c r="BB23" s="90"/>
-      <c r="BC23" s="90"/>
+      <c r="AV23" s="73"/>
+      <c r="AW23" s="73"/>
+      <c r="AX23" s="73"/>
+      <c r="AY23" s="73"/>
+      <c r="AZ23" s="73"/>
+      <c r="BA23" s="73"/>
+      <c r="BB23" s="73"/>
+      <c r="BC23" s="73"/>
       <c r="BD23" s="37"/>
       <c r="BE23" s="37"/>
       <c r="BF23" s="37"/>
@@ -5202,19 +5174,19 @@
     </row>
     <row r="24" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="13"/>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="78">
-        <v>0</v>
-      </c>
-      <c r="E24" s="79">
+      <c r="D24" s="77">
+        <v>1</v>
+      </c>
+      <c r="E24" s="78">
         <v>45709</v>
       </c>
-      <c r="F24" s="79">
+      <c r="F24" s="78">
         <v>45716</v>
       </c>
       <c r="G24" s="17"/>
@@ -5258,14 +5230,14 @@
       <c r="AS24" s="37"/>
       <c r="AT24" s="37"/>
       <c r="AU24" s="37"/>
-      <c r="AV24" s="84"/>
-      <c r="AW24" s="84"/>
-      <c r="AX24" s="84"/>
-      <c r="AY24" s="84"/>
-      <c r="AZ24" s="84"/>
-      <c r="BA24" s="84"/>
-      <c r="BB24" s="84"/>
-      <c r="BC24" s="84"/>
+      <c r="AV24" s="74"/>
+      <c r="AW24" s="74"/>
+      <c r="AX24" s="74"/>
+      <c r="AY24" s="74"/>
+      <c r="AZ24" s="74"/>
+      <c r="BA24" s="74"/>
+      <c r="BB24" s="74"/>
+      <c r="BC24" s="74"/>
       <c r="BD24" s="37"/>
       <c r="BE24" s="37"/>
       <c r="BF24" s="37"/>
@@ -5341,7 +5313,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="36">
         <v>45709</v>
@@ -5390,14 +5362,14 @@
       <c r="AS25" s="37"/>
       <c r="AT25" s="37"/>
       <c r="AU25" s="37"/>
-      <c r="AV25" s="89"/>
-      <c r="AW25" s="89"/>
-      <c r="AX25" s="89"/>
-      <c r="AY25" s="89"/>
-      <c r="AZ25" s="89"/>
-      <c r="BA25" s="89"/>
-      <c r="BB25" s="89"/>
-      <c r="BC25" s="89"/>
+      <c r="AV25" s="87"/>
+      <c r="AW25" s="87"/>
+      <c r="AX25" s="87"/>
+      <c r="AY25" s="87"/>
+      <c r="AZ25" s="87"/>
+      <c r="BA25" s="87"/>
+      <c r="BB25" s="87"/>
+      <c r="BC25" s="87"/>
       <c r="BD25" s="37"/>
       <c r="BE25" s="37"/>
       <c r="BF25" s="37"/>
@@ -5473,7 +5445,7 @@
         <v>33</v>
       </c>
       <c r="D26" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="61">
         <v>45716</v>
@@ -5529,7 +5501,7 @@
       <c r="AZ26" s="37"/>
       <c r="BA26" s="37"/>
       <c r="BB26" s="37"/>
-      <c r="BC26" s="63"/>
+      <c r="BC26" s="62"/>
       <c r="BD26" s="37"/>
       <c r="BE26" s="37"/>
       <c r="BF26" s="37"/>
@@ -5605,7 +5577,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="39">
         <f>F23</f>
@@ -5732,20 +5704,20 @@
     </row>
     <row r="28" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="13"/>
-      <c r="B28" s="85" t="s">
+      <c r="B28" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="87">
-        <v>0</v>
-      </c>
-      <c r="E28" s="88">
+      <c r="D28" s="85">
+        <v>1</v>
+      </c>
+      <c r="E28" s="86">
         <f>F26</f>
         <v>45716</v>
       </c>
-      <c r="F28" s="88">
+      <c r="F28" s="86">
         <f>E28+7</f>
         <v>45723</v>
       </c>
@@ -5797,14 +5769,14 @@
       <c r="AZ28" s="37"/>
       <c r="BA28" s="37"/>
       <c r="BB28" s="37"/>
-      <c r="BC28" s="90"/>
-      <c r="BD28" s="90"/>
-      <c r="BE28" s="90"/>
-      <c r="BF28" s="90"/>
-      <c r="BG28" s="90"/>
-      <c r="BH28" s="90"/>
-      <c r="BI28" s="90"/>
-      <c r="BJ28" s="90"/>
+      <c r="BC28" s="73"/>
+      <c r="BD28" s="73"/>
+      <c r="BE28" s="73"/>
+      <c r="BF28" s="73"/>
+      <c r="BG28" s="73"/>
+      <c r="BH28" s="73"/>
+      <c r="BI28" s="73"/>
+      <c r="BJ28" s="73"/>
       <c r="BK28" s="37"/>
       <c r="BL28" s="37"/>
       <c r="BM28" s="37"/>
@@ -5866,19 +5838,19 @@
     </row>
     <row r="29" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="13"/>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="82">
-        <v>0</v>
-      </c>
-      <c r="E29" s="83">
+      <c r="D29" s="81">
+        <v>1</v>
+      </c>
+      <c r="E29" s="82">
         <v>45716</v>
       </c>
-      <c r="F29" s="83">
+      <c r="F29" s="82">
         <v>45723</v>
       </c>
       <c r="G29" s="17"/>
@@ -5929,14 +5901,14 @@
       <c r="AZ29" s="37"/>
       <c r="BA29" s="37"/>
       <c r="BB29" s="37"/>
-      <c r="BC29" s="84"/>
-      <c r="BD29" s="84"/>
-      <c r="BE29" s="84"/>
-      <c r="BF29" s="84"/>
-      <c r="BG29" s="84"/>
-      <c r="BH29" s="84"/>
-      <c r="BI29" s="84"/>
-      <c r="BJ29" s="84"/>
+      <c r="BC29" s="74"/>
+      <c r="BD29" s="74"/>
+      <c r="BE29" s="74"/>
+      <c r="BF29" s="74"/>
+      <c r="BG29" s="74"/>
+      <c r="BH29" s="74"/>
+      <c r="BI29" s="74"/>
+      <c r="BJ29" s="74"/>
       <c r="BK29" s="37"/>
       <c r="BL29" s="37"/>
       <c r="BM29" s="37"/>
@@ -5998,20 +5970,20 @@
     </row>
     <row r="30" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="13"/>
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="82">
-        <v>0</v>
-      </c>
-      <c r="E30" s="83">
+      <c r="D30" s="81">
+        <v>1</v>
+      </c>
+      <c r="E30" s="82">
         <f>F27</f>
         <v>45723</v>
       </c>
-      <c r="F30" s="83">
+      <c r="F30" s="82">
         <f>E30+7</f>
         <v>45730</v>
       </c>
@@ -6070,14 +6042,14 @@
       <c r="BG30" s="37"/>
       <c r="BH30" s="37"/>
       <c r="BI30" s="37"/>
-      <c r="BJ30" s="84"/>
-      <c r="BK30" s="84"/>
-      <c r="BL30" s="84"/>
-      <c r="BM30" s="84"/>
-      <c r="BN30" s="84"/>
-      <c r="BO30" s="84"/>
-      <c r="BP30" s="84"/>
-      <c r="BQ30" s="84"/>
+      <c r="BJ30" s="74"/>
+      <c r="BK30" s="74"/>
+      <c r="BL30" s="74"/>
+      <c r="BM30" s="74"/>
+      <c r="BN30" s="74"/>
+      <c r="BO30" s="74"/>
+      <c r="BP30" s="74"/>
+      <c r="BQ30" s="74"/>
       <c r="BR30" s="37"/>
       <c r="BS30" s="37"/>
       <c r="BT30" s="37"/>
@@ -6132,19 +6104,19 @@
     </row>
     <row r="31" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="13"/>
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="87">
-        <v>0</v>
-      </c>
-      <c r="E31" s="88">
+      <c r="D31" s="85">
+        <v>1</v>
+      </c>
+      <c r="E31" s="86">
         <v>45723</v>
       </c>
-      <c r="F31" s="88">
+      <c r="F31" s="86">
         <v>45730</v>
       </c>
       <c r="G31" s="17"/>
@@ -6202,14 +6174,14 @@
       <c r="BG31" s="37"/>
       <c r="BH31" s="37"/>
       <c r="BI31" s="37"/>
-      <c r="BJ31" s="90"/>
-      <c r="BK31" s="90"/>
-      <c r="BL31" s="90"/>
-      <c r="BM31" s="90"/>
-      <c r="BN31" s="90"/>
-      <c r="BO31" s="90"/>
-      <c r="BP31" s="90"/>
-      <c r="BQ31" s="90"/>
+      <c r="BJ31" s="73"/>
+      <c r="BK31" s="73"/>
+      <c r="BL31" s="73"/>
+      <c r="BM31" s="73"/>
+      <c r="BN31" s="73"/>
+      <c r="BO31" s="73"/>
+      <c r="BP31" s="73"/>
+      <c r="BQ31" s="73"/>
       <c r="BR31" s="37"/>
       <c r="BS31" s="37"/>
       <c r="BT31" s="37"/>
@@ -6271,7 +6243,7 @@
         <v>39</v>
       </c>
       <c r="D32" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="39">
         <v>45723</v>
@@ -6403,7 +6375,7 @@
         <v>39</v>
       </c>
       <c r="D33" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="39">
         <v>45730</v>
@@ -6528,19 +6500,19 @@
     </row>
     <row r="34" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="13"/>
-      <c r="B34" s="80" t="s">
+      <c r="B34" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="81" t="s">
+      <c r="C34" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="82">
-        <v>0</v>
-      </c>
-      <c r="E34" s="83">
+      <c r="D34" s="81">
+        <v>1</v>
+      </c>
+      <c r="E34" s="82">
         <v>45730</v>
       </c>
-      <c r="F34" s="83">
+      <c r="F34" s="82">
         <v>45737</v>
       </c>
       <c r="G34" s="17"/>
@@ -6605,14 +6577,14 @@
       <c r="BN34" s="37"/>
       <c r="BO34" s="37"/>
       <c r="BP34" s="37"/>
-      <c r="BQ34" s="84"/>
-      <c r="BR34" s="84"/>
-      <c r="BS34" s="84"/>
-      <c r="BT34" s="84"/>
-      <c r="BU34" s="84"/>
-      <c r="BV34" s="84"/>
-      <c r="BW34" s="84"/>
-      <c r="BX34" s="84"/>
+      <c r="BQ34" s="74"/>
+      <c r="BR34" s="74"/>
+      <c r="BS34" s="74"/>
+      <c r="BT34" s="74"/>
+      <c r="BU34" s="74"/>
+      <c r="BV34" s="74"/>
+      <c r="BW34" s="74"/>
+      <c r="BX34" s="74"/>
       <c r="BY34" s="37"/>
       <c r="BZ34" s="37"/>
       <c r="CA34" s="37"/>
@@ -6660,19 +6632,19 @@
     </row>
     <row r="35" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="13"/>
-      <c r="B35" s="85" t="s">
+      <c r="B35" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C35" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="87">
-        <v>0</v>
-      </c>
-      <c r="E35" s="88">
+      <c r="D35" s="85">
+        <v>1</v>
+      </c>
+      <c r="E35" s="86">
         <v>45730</v>
       </c>
-      <c r="F35" s="88">
+      <c r="F35" s="86">
         <v>45737</v>
       </c>
       <c r="G35" s="17"/>
@@ -6737,14 +6709,14 @@
       <c r="BN35" s="37"/>
       <c r="BO35" s="37"/>
       <c r="BP35" s="37"/>
-      <c r="BQ35" s="90"/>
-      <c r="BR35" s="90"/>
-      <c r="BS35" s="90"/>
-      <c r="BT35" s="90"/>
-      <c r="BU35" s="90"/>
-      <c r="BV35" s="90"/>
-      <c r="BW35" s="90"/>
-      <c r="BX35" s="90"/>
+      <c r="BQ35" s="73"/>
+      <c r="BR35" s="73"/>
+      <c r="BS35" s="73"/>
+      <c r="BT35" s="73"/>
+      <c r="BU35" s="73"/>
+      <c r="BV35" s="73"/>
+      <c r="BW35" s="73"/>
+      <c r="BX35" s="73"/>
       <c r="BY35" s="37"/>
       <c r="BZ35" s="37"/>
       <c r="CA35" s="37"/>
@@ -6799,7 +6771,7 @@
         <v>39</v>
       </c>
       <c r="D36" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="39">
         <f>F30</f>
@@ -6933,7 +6905,7 @@
         <v>33</v>
       </c>
       <c r="D37" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="61">
         <v>45737</v>
@@ -7010,7 +6982,7 @@
       <c r="BU37" s="37"/>
       <c r="BV37" s="37"/>
       <c r="BW37" s="37"/>
-      <c r="BX37" s="63"/>
+      <c r="BX37" s="62"/>
       <c r="BY37" s="37"/>
       <c r="BZ37" s="37"/>
       <c r="CA37" s="37"/>
@@ -7065,7 +7037,7 @@
         <v>39</v>
       </c>
       <c r="D38" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="36">
         <v>45737</v>
@@ -7190,19 +7162,19 @@
     </row>
     <row r="39" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="13"/>
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="71" t="s">
+      <c r="C39" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="72">
-        <v>0</v>
-      </c>
-      <c r="E39" s="73">
+      <c r="D39" s="71">
+        <v>1</v>
+      </c>
+      <c r="E39" s="72">
         <v>45737</v>
       </c>
-      <c r="F39" s="73">
+      <c r="F39" s="72">
         <v>45744</v>
       </c>
       <c r="G39" s="17"/>
@@ -7274,14 +7246,14 @@
       <c r="BU39" s="37"/>
       <c r="BV39" s="37"/>
       <c r="BW39" s="37"/>
-      <c r="BX39" s="90"/>
-      <c r="BY39" s="90"/>
-      <c r="BZ39" s="90"/>
-      <c r="CA39" s="90"/>
-      <c r="CB39" s="90"/>
-      <c r="CC39" s="90"/>
-      <c r="CD39" s="90"/>
-      <c r="CE39" s="90"/>
+      <c r="BX39" s="73"/>
+      <c r="BY39" s="73"/>
+      <c r="BZ39" s="73"/>
+      <c r="CA39" s="73"/>
+      <c r="CB39" s="73"/>
+      <c r="CC39" s="73"/>
+      <c r="CD39" s="73"/>
+      <c r="CE39" s="73"/>
       <c r="CF39" s="37"/>
       <c r="CG39" s="37"/>
       <c r="CH39" s="37"/>
@@ -7322,20 +7294,20 @@
     </row>
     <row r="40" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="13"/>
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="81" t="s">
+      <c r="C40" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="82">
-        <v>0</v>
-      </c>
-      <c r="E40" s="83">
+      <c r="D40" s="81">
+        <v>1</v>
+      </c>
+      <c r="E40" s="82">
         <f>F36</f>
         <v>45737</v>
       </c>
-      <c r="F40" s="83">
+      <c r="F40" s="82">
         <f>E40+7</f>
         <v>45744</v>
       </c>
@@ -7408,14 +7380,14 @@
       <c r="BU40" s="37"/>
       <c r="BV40" s="37"/>
       <c r="BW40" s="37"/>
-      <c r="BX40" s="84"/>
-      <c r="BY40" s="84"/>
-      <c r="BZ40" s="84"/>
-      <c r="CA40" s="84"/>
-      <c r="CB40" s="84"/>
-      <c r="CC40" s="84"/>
-      <c r="CD40" s="84"/>
-      <c r="CE40" s="84"/>
+      <c r="BX40" s="74"/>
+      <c r="BY40" s="74"/>
+      <c r="BZ40" s="74"/>
+      <c r="CA40" s="74"/>
+      <c r="CB40" s="74"/>
+      <c r="CC40" s="74"/>
+      <c r="CD40" s="74"/>
+      <c r="CE40" s="74"/>
       <c r="CF40" s="37"/>
       <c r="CG40" s="37"/>
       <c r="CH40" s="37"/>
@@ -7463,7 +7435,7 @@
         <v>33</v>
       </c>
       <c r="D41" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="61">
         <v>45744</v>
@@ -7546,7 +7518,7 @@
       <c r="CB41" s="37"/>
       <c r="CC41" s="40"/>
       <c r="CD41" s="37"/>
-      <c r="CE41" s="63"/>
+      <c r="CE41" s="62"/>
       <c r="CF41" s="37"/>
       <c r="CG41" s="37"/>
       <c r="CH41" s="37"/>
@@ -7587,20 +7559,20 @@
     </row>
     <row r="42" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="13"/>
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="81" t="s">
+      <c r="C42" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="82">
-        <v>0</v>
-      </c>
-      <c r="E42" s="83">
+      <c r="D42" s="81">
+        <v>1</v>
+      </c>
+      <c r="E42" s="82">
         <f>F40</f>
         <v>45744</v>
       </c>
-      <c r="F42" s="83">
+      <c r="F42" s="82">
         <f>E42+7</f>
         <v>45751</v>
       </c>
@@ -7679,14 +7651,14 @@
       <c r="CB42" s="37"/>
       <c r="CC42" s="40"/>
       <c r="CD42" s="37"/>
-      <c r="CE42" s="84"/>
-      <c r="CF42" s="84"/>
-      <c r="CG42" s="84"/>
-      <c r="CH42" s="84"/>
-      <c r="CI42" s="84"/>
-      <c r="CJ42" s="84"/>
-      <c r="CK42" s="84"/>
-      <c r="CL42" s="84"/>
+      <c r="CE42" s="74"/>
+      <c r="CF42" s="74"/>
+      <c r="CG42" s="74"/>
+      <c r="CH42" s="74"/>
+      <c r="CI42" s="74"/>
+      <c r="CJ42" s="74"/>
+      <c r="CK42" s="74"/>
+      <c r="CL42" s="74"/>
       <c r="CM42" s="37"/>
       <c r="CN42" s="37"/>
       <c r="CO42" s="37"/>
@@ -7727,7 +7699,7 @@
         <v>39</v>
       </c>
       <c r="D43" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="39">
         <v>45744</v>
@@ -7852,20 +7824,20 @@
     </row>
     <row r="44" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="13"/>
-      <c r="B44" s="85" t="s">
+      <c r="B44" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="87">
-        <v>0</v>
-      </c>
-      <c r="E44" s="88">
+      <c r="D44" s="85">
+        <v>1</v>
+      </c>
+      <c r="E44" s="86">
         <f>F42</f>
         <v>45751</v>
       </c>
-      <c r="F44" s="88">
+      <c r="F44" s="86">
         <f>E44+7</f>
         <v>45758</v>
       </c>
@@ -7952,14 +7924,14 @@
       <c r="CI44" s="37"/>
       <c r="CJ44" s="37"/>
       <c r="CK44" s="37"/>
-      <c r="CL44" s="90"/>
-      <c r="CM44" s="90"/>
-      <c r="CN44" s="90"/>
-      <c r="CO44" s="90"/>
-      <c r="CP44" s="90"/>
-      <c r="CQ44" s="90"/>
-      <c r="CR44" s="90"/>
-      <c r="CS44" s="90"/>
+      <c r="CL44" s="73"/>
+      <c r="CM44" s="73"/>
+      <c r="CN44" s="73"/>
+      <c r="CO44" s="73"/>
+      <c r="CP44" s="73"/>
+      <c r="CQ44" s="73"/>
+      <c r="CR44" s="73"/>
+      <c r="CS44" s="73"/>
       <c r="CT44" s="37"/>
       <c r="CU44" s="37"/>
       <c r="CV44" s="37"/>
@@ -7993,7 +7965,7 @@
         <v>33</v>
       </c>
       <c r="D45" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="61">
         <v>45758</v>
@@ -8091,7 +8063,7 @@
       <c r="CP45" s="37"/>
       <c r="CQ45" s="40"/>
       <c r="CR45" s="37"/>
-      <c r="CS45" s="63"/>
+      <c r="CS45" s="62"/>
       <c r="CT45" s="37"/>
       <c r="CU45" s="37"/>
       <c r="CV45" s="37"/>
@@ -8118,20 +8090,20 @@
     </row>
     <row r="46" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="13"/>
-      <c r="B46" s="80" t="s">
+      <c r="B46" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="82">
-        <v>0</v>
-      </c>
-      <c r="E46" s="83">
+      <c r="D46" s="81">
+        <v>1</v>
+      </c>
+      <c r="E46" s="82">
         <f>F44</f>
         <v>45758</v>
       </c>
-      <c r="F46" s="83">
+      <c r="F46" s="82">
         <f>E46+7</f>
         <v>45765</v>
       </c>
@@ -8225,14 +8197,14 @@
       <c r="CP46" s="37"/>
       <c r="CQ46" s="40"/>
       <c r="CR46" s="37"/>
-      <c r="CS46" s="84"/>
-      <c r="CT46" s="84"/>
-      <c r="CU46" s="84"/>
-      <c r="CV46" s="84"/>
-      <c r="CW46" s="84"/>
-      <c r="CX46" s="84"/>
-      <c r="CY46" s="84"/>
-      <c r="CZ46" s="84"/>
+      <c r="CS46" s="74"/>
+      <c r="CT46" s="74"/>
+      <c r="CU46" s="74"/>
+      <c r="CV46" s="74"/>
+      <c r="CW46" s="74"/>
+      <c r="CX46" s="74"/>
+      <c r="CY46" s="74"/>
+      <c r="CZ46" s="74"/>
       <c r="DA46" s="37"/>
       <c r="DB46" s="37"/>
       <c r="DC46" s="37"/>
@@ -8252,20 +8224,20 @@
     </row>
     <row r="47" spans="1:120" s="34" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="13"/>
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="86" t="s">
+      <c r="C47" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="87">
-        <v>0</v>
-      </c>
-      <c r="E47" s="88">
+      <c r="D47" s="85">
+        <v>1</v>
+      </c>
+      <c r="E47" s="86">
         <f>F46</f>
         <v>45765</v>
       </c>
-      <c r="F47" s="88">
+      <c r="F47" s="86">
         <f>E47+7</f>
         <v>45772</v>
       </c>
@@ -8366,14 +8338,14 @@
       <c r="CW47" s="37"/>
       <c r="CX47" s="37"/>
       <c r="CY47" s="37"/>
-      <c r="CZ47" s="90"/>
-      <c r="DA47" s="90"/>
-      <c r="DB47" s="90"/>
-      <c r="DC47" s="90"/>
-      <c r="DD47" s="90"/>
-      <c r="DE47" s="90"/>
-      <c r="DF47" s="90"/>
-      <c r="DG47" s="90"/>
+      <c r="CZ47" s="73"/>
+      <c r="DA47" s="73"/>
+      <c r="DB47" s="73"/>
+      <c r="DC47" s="73"/>
+      <c r="DD47" s="73"/>
+      <c r="DE47" s="73"/>
+      <c r="DF47" s="73"/>
+      <c r="DG47" s="73"/>
       <c r="DH47" s="37"/>
       <c r="DI47" s="37"/>
       <c r="DJ47" s="37"/>
@@ -8393,7 +8365,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="61">
         <v>45775</v>
@@ -8508,7 +8480,7 @@
       <c r="DG48" s="37"/>
       <c r="DH48" s="37"/>
       <c r="DI48" s="37"/>
-      <c r="DJ48" s="63"/>
+      <c r="DJ48" s="62"/>
       <c r="DK48" s="37"/>
       <c r="DL48" s="40"/>
       <c r="DM48" s="37"/>
@@ -8525,7 +8497,7 @@
         <v>39</v>
       </c>
       <c r="D49" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="39">
         <f>F47</f>
@@ -8781,7 +8753,7 @@
       <c r="DK50" s="37"/>
       <c r="DL50" s="37"/>
       <c r="DM50" s="37"/>
-      <c r="DN50" s="63"/>
+      <c r="DN50" s="62"/>
       <c r="DO50" s="37"/>
       <c r="DP50" s="37"/>
     </row>
@@ -8924,17 +8896,14 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -8943,14 +8912,17 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D51">
     <cfRule type="dataBar" priority="50">
@@ -9223,23 +9195,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9555,29 +9516,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9604,9 +9565,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>